<commit_message>
Vehicle price and MPNVbT edits
</commit_message>
<xml_diff>
--- a/InputData/trans/MPNVbT/Max Perc New Veh by Technology.xlsx
+++ b/InputData/trans/MPNVbT/Max Perc New Veh by Technology.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-india\InputData\trans\MPNVbT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-india\InputData\trans\MPNVbT\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <sheet name="MPNVbT-motorbikes-psgr" sheetId="17" r:id="rId16"/>
     <sheet name="MPNVbT-motorbikes-frgt" sheetId="18" r:id="rId17"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -678,7 +678,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2011,7 +2010,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
@@ -10140,135 +10139,135 @@
       </c>
       <c r="C2">
         <f>'India Data'!I85</f>
-        <v>3.6056435541586503E-2</v>
+        <v>3.9032481401698134E-2</v>
       </c>
       <c r="D2">
         <f>'India Data'!J85</f>
-        <v>3.6841900503310654E-2</v>
+        <v>4.0831449539840532E-2</v>
       </c>
       <c r="E2">
         <f>'India Data'!K85</f>
-        <v>3.788515075294395E-2</v>
+        <v>4.3220829143839373E-2</v>
       </c>
       <c r="F2">
         <f>'India Data'!L85</f>
-        <v>3.9263257756892135E-2</v>
+        <v>4.6377138733527154E-2</v>
       </c>
       <c r="G2">
         <f>'India Data'!M85</f>
-        <v>4.1070652641625835E-2</v>
+        <v>5.0516656050175315E-2</v>
       </c>
       <c r="H2">
         <f>'India Data'!N85</f>
-        <v>4.3418825967418473E-2</v>
+        <v>5.5894730441506828E-2</v>
       </c>
       <c r="I2">
         <f>'India Data'!O85</f>
-        <v>4.6432505463989998E-2</v>
+        <v>6.2797028643331934E-2</v>
       </c>
       <c r="J2">
         <f>'India Data'!P85</f>
-        <v>5.0240186294681702E-2</v>
+        <v>7.1517846029754875E-2</v>
       </c>
       <c r="K2">
         <f>'India Data'!Q85</f>
-        <v>5.4956967142488919E-2</v>
+        <v>8.2320795713442363E-2</v>
       </c>
       <c r="L2">
         <f>'India Data'!R85</f>
-        <v>6.0658993918239194E-2</v>
+        <v>9.5380276393386546E-2</v>
       </c>
       <c r="M2">
         <f>'India Data'!S85</f>
-        <v>6.7352120319843278E-2</v>
+        <v>0.1107096949260927</v>
       </c>
       <c r="N2">
         <f>'India Data'!T85</f>
-        <v>7.4942454401251274E-2</v>
+        <v>0.12809400846738195</v>
       </c>
       <c r="O2">
         <f>'India Data'!U85</f>
-        <v>8.3221057420644631E-2</v>
+        <v>0.14705467989889578</v>
       </c>
       <c r="P2">
         <f>'India Data'!V85</f>
-        <v>9.1874999999999984E-2</v>
+        <v>0.166875</v>
       </c>
       <c r="Q2">
         <f>'India Data'!W85</f>
-        <v>0.10052894257935535</v>
+        <v>0.18669532010110421</v>
       </c>
       <c r="R2">
         <f>'India Data'!X85</f>
-        <v>0.1088075455987487</v>
+        <v>0.20565599153261802</v>
       </c>
       <c r="S2">
         <f>'India Data'!Y85</f>
-        <v>0.11639787968015669</v>
+        <v>0.22304030507390729</v>
       </c>
       <c r="T2">
         <f>'India Data'!Z85</f>
-        <v>0.1230910060817608</v>
+        <v>0.23836972360661343</v>
       </c>
       <c r="U2">
         <f>'India Data'!AA85</f>
-        <v>0.12879303285751106</v>
+        <v>0.25142920428655757</v>
       </c>
       <c r="V2">
         <f>'India Data'!AB85</f>
-        <v>0.13350981370531828</v>
+        <v>0.26223215397024513</v>
       </c>
       <c r="W2">
         <f>'India Data'!AC85</f>
-        <v>0.13731749453601</v>
+        <v>0.27095297135666802</v>
       </c>
       <c r="X2">
         <f>'India Data'!AD85</f>
-        <v>0.14033117403258152</v>
+        <v>0.27785526955849316</v>
       </c>
       <c r="Y2">
         <f>'India Data'!AE85</f>
-        <v>0.14267934735837415</v>
+        <v>0.28323334394982469</v>
       </c>
       <c r="Z2">
         <f>'India Data'!AF85</f>
-        <v>0.14448674224310787</v>
+        <v>0.28737286126647288</v>
       </c>
       <c r="AA2">
         <f>'India Data'!AG85</f>
-        <v>0.14586484924705603</v>
+        <v>0.29052917085616059</v>
       </c>
       <c r="AB2">
         <f>'India Data'!AH85</f>
-        <v>0.14690809949668931</v>
+        <v>0.29291855046015941</v>
       </c>
       <c r="AC2">
         <f>'India Data'!AI85</f>
-        <v>0.14769356445841347</v>
+        <v>0.29471751859830186</v>
       </c>
       <c r="AD2">
         <f>'India Data'!AJ85</f>
-        <v>0.14828251881565699</v>
+        <v>0.29606641406166606</v>
       </c>
       <c r="AE2">
         <f>'India Data'!AK85</f>
-        <v>0.14872276791919353</v>
+        <v>0.29707472652460454</v>
       </c>
       <c r="AF2">
         <f>'India Data'!AL85</f>
-        <v>0.14905110110344516</v>
+        <v>0.29782671543047118</v>
       </c>
       <c r="AG2">
         <f>'India Data'!AM85</f>
-        <v>0.14929554807660333</v>
+        <v>0.29838657785286571</v>
       </c>
       <c r="AH2">
         <f>'India Data'!AN85</f>
-        <v>0.14947730824504057</v>
+        <v>0.29880286727089939</v>
       </c>
       <c r="AI2">
         <f>'India Data'!AO85</f>
-        <v>0.14961232865051319</v>
+        <v>0.29911210755440121</v>
       </c>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.45">
@@ -10704,135 +10703,135 @@
       </c>
       <c r="C6">
         <f>'India Data'!I89</f>
-        <v>1.488022930055813E-3</v>
+        <v>2.9760458601116261E-3</v>
       </c>
       <c r="D6">
         <f>'India Data'!J89</f>
-        <v>1.9947745182649396E-3</v>
+        <v>3.9895490365298792E-3</v>
       </c>
       <c r="E6">
         <f>'India Data'!K89</f>
-        <v>2.6678391954477131E-3</v>
+        <v>5.3356783908954262E-3</v>
       </c>
       <c r="F6">
         <f>'India Data'!L89</f>
-        <v>3.5569404883175086E-3</v>
+        <v>7.1138809766350172E-3</v>
       </c>
       <c r="G6">
         <f>'India Data'!M89</f>
-        <v>4.7230017042747376E-3</v>
+        <v>9.4460034085494752E-3</v>
       </c>
       <c r="H6">
         <f>'India Data'!N89</f>
-        <v>6.2379522370441774E-3</v>
+        <v>1.2475904474088355E-2</v>
       </c>
       <c r="I6">
         <f>'India Data'!O89</f>
-        <v>8.182261589670968E-3</v>
+        <v>1.6364523179341936E-2</v>
       </c>
       <c r="J6">
         <f>'India Data'!P89</f>
-        <v>1.0638829867536587E-2</v>
+        <v>2.1277659735073173E-2</v>
       </c>
       <c r="K6">
         <f>'India Data'!Q89</f>
-        <v>1.3681914285476725E-2</v>
+        <v>2.7363828570953451E-2</v>
       </c>
       <c r="L6">
         <f>'India Data'!R89</f>
-        <v>1.7360641237573676E-2</v>
+        <v>3.4721282475147351E-2</v>
       </c>
       <c r="M6">
         <f>'India Data'!S89</f>
-        <v>2.1678787303124704E-2</v>
+        <v>4.3357574606249408E-2</v>
       </c>
       <c r="N6">
         <f>'India Data'!T89</f>
-        <v>2.657577703306534E-2</v>
+        <v>5.3151554066130681E-2</v>
       </c>
       <c r="O6">
         <f>'India Data'!U89</f>
-        <v>3.1916811239125577E-2</v>
+        <v>6.3833622478251154E-2</v>
       </c>
       <c r="P6">
         <f>'India Data'!V89</f>
-        <v>3.7499999999999999E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="Q6">
         <f>'India Data'!W89</f>
-        <v>4.3083188760874427E-2</v>
+        <v>8.6166377521748855E-2</v>
       </c>
       <c r="R6">
         <f>'India Data'!X89</f>
-        <v>4.8424222966934653E-2</v>
+        <v>9.6848445933869307E-2</v>
       </c>
       <c r="S6">
         <f>'India Data'!Y89</f>
-        <v>5.3321212696875293E-2</v>
+        <v>0.10664242539375059</v>
       </c>
       <c r="T6">
         <f>'India Data'!Z89</f>
-        <v>5.7639358762426318E-2</v>
+        <v>0.11527871752485264</v>
       </c>
       <c r="U6">
         <f>'India Data'!AA89</f>
-        <v>6.1318085714523268E-2</v>
+        <v>0.12263617142904654</v>
       </c>
       <c r="V6">
         <f>'India Data'!AB89</f>
-        <v>6.4361170132463424E-2</v>
+        <v>0.12872234026492685</v>
       </c>
       <c r="W6">
         <f>'India Data'!AC89</f>
-        <v>6.6817738410329036E-2</v>
+        <v>0.13363547682065807</v>
       </c>
       <c r="X6">
         <f>'India Data'!AD89</f>
-        <v>6.8762047762955816E-2</v>
+        <v>0.13752409552591163</v>
       </c>
       <c r="Y6">
         <f>'India Data'!AE89</f>
-        <v>7.0276998295725257E-2</v>
+        <v>0.14055399659145051</v>
       </c>
       <c r="Z6">
         <f>'India Data'!AF89</f>
-        <v>7.1443059511682491E-2</v>
+        <v>0.14288611902336498</v>
       </c>
       <c r="AA6">
         <f>'India Data'!AG89</f>
-        <v>7.2332160804552292E-2</v>
+        <v>0.14466432160910458</v>
       </c>
       <c r="AB6">
         <f>'India Data'!AH89</f>
-        <v>7.3005225481735048E-2</v>
+        <v>0.1460104509634701</v>
       </c>
       <c r="AC6">
         <f>'India Data'!AI89</f>
-        <v>7.3511977069944182E-2</v>
+        <v>0.14702395413988836</v>
       </c>
       <c r="AD6">
         <f>'India Data'!AJ89</f>
-        <v>7.3891947623004522E-2</v>
+        <v>0.14778389524600904</v>
       </c>
       <c r="AE6">
         <f>'India Data'!AK89</f>
-        <v>7.4175979302705516E-2</v>
+        <v>0.14835195860541103</v>
       </c>
       <c r="AF6">
         <f>'India Data'!AL89</f>
-        <v>7.4387807163513009E-2</v>
+        <v>0.14877561432702602</v>
       </c>
       <c r="AG6">
         <f>'India Data'!AM89</f>
-        <v>7.4545514888131187E-2</v>
+        <v>0.14909102977626237</v>
       </c>
       <c r="AH6">
         <f>'India Data'!AN89</f>
-        <v>7.4662779512929406E-2</v>
+        <v>0.14932555902585881</v>
       </c>
       <c r="AI6">
         <f>'India Data'!AO89</f>
-        <v>7.4749889451943996E-2</v>
+        <v>0.14949977890388799</v>
       </c>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.45">
@@ -11745,8 +11744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP91"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -13079,7 +13078,6 @@
         <v>0</v>
       </c>
       <c r="E15" s="10">
-        <f>E8*'India Assumptions'!$A$31</f>
         <v>0.15</v>
       </c>
       <c r="F15" s="15" t="str">
@@ -13231,157 +13229,157 @@
       <c r="C16" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="10">
-        <f>'SYVbT-freight'!C$2/SUM('SYVbT-freight'!B$2:H$2)</f>
-        <v>0</v>
+      <c r="D16" s="4">
+        <f>D9</f>
+        <v>2.6163522012578631E-2</v>
       </c>
       <c r="E16" s="10">
         <f>MIN(1,D16*'India Assumptions'!$A$10)</f>
-        <v>0</v>
+        <v>1.3081761006289315E-2</v>
       </c>
       <c r="F16" s="15" t="str">
         <f t="shared" si="4"/>
-        <v>n/a</v>
+        <v>linear</v>
       </c>
       <c r="H16" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2.6163522012578631E-2</v>
       </c>
       <c r="I16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($H$7:I$7)+$I$4))),TREND($D16:$E16,$D$7:$E$7,I$7))</f>
-        <v>0</v>
+        <v>2.5778764335922966E-2</v>
       </c>
       <c r="J16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($H$7:J$7)+$I$4))),TREND($D16:$E16,$D$7:$E$7,J$7))</f>
-        <v>0</v>
+        <v>2.5394006659267387E-2</v>
       </c>
       <c r="K16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($H$7:K$7)+$I$4))),TREND($D16:$E16,$D$7:$E$7,K$7))</f>
-        <v>0</v>
+        <v>2.5009248982611809E-2</v>
       </c>
       <c r="L16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($H$7:L$7)+$I$4))),TREND($D16:$E16,$D$7:$E$7,L$7))</f>
-        <v>0</v>
+        <v>2.4624491305956231E-2</v>
       </c>
       <c r="M16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($H$7:M$7)+$I$4))),TREND($D16:$E16,$D$7:$E$7,M$7))</f>
-        <v>0</v>
+        <v>2.4239733629300764E-2</v>
       </c>
       <c r="N16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($H$7:N$7)+$I$4))),TREND($D16:$E16,$D$7:$E$7,N$7))</f>
-        <v>0</v>
+        <v>2.3854975952645185E-2</v>
       </c>
       <c r="O16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($H$7:O$7)+$I$4))),TREND($D16:$E16,$D$7:$E$7,O$7))</f>
-        <v>0</v>
+        <v>2.3470218275989607E-2</v>
       </c>
       <c r="P16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($H$7:P$7)+$I$4))),TREND($D16:$E16,$D$7:$E$7,P$7))</f>
-        <v>0</v>
+        <v>2.3085460599334029E-2</v>
       </c>
       <c r="Q16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($H$7:Q$7)+$I$4))),TREND($D16:$E16,$D$7:$E$7,Q$7))</f>
-        <v>0</v>
+        <v>2.2700702922678451E-2</v>
       </c>
       <c r="R16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($H$7:R$7)+$I$4))),TREND($D16:$E16,$D$7:$E$7,R$7))</f>
-        <v>0</v>
+        <v>2.2315945246022872E-2</v>
       </c>
       <c r="S16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($H$7:S$7)+$I$4))),TREND($D16:$E16,$D$7:$E$7,S$7))</f>
-        <v>0</v>
+        <v>2.1931187569367294E-2</v>
       </c>
       <c r="T16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($H$7:T$7)+$I$4))),TREND($D16:$E16,$D$7:$E$7,T$7))</f>
-        <v>0</v>
+        <v>2.1546429892711716E-2</v>
       </c>
       <c r="U16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($H$7:U$7)+$I$4))),TREND($D16:$E16,$D$7:$E$7,U$7))</f>
-        <v>0</v>
+        <v>2.1161672216056138E-2</v>
       </c>
       <c r="V16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($H$7:V$7)+$I$4))),TREND($D16:$E16,$D$7:$E$7,V$7))</f>
-        <v>0</v>
+        <v>2.0776914539400559E-2</v>
       </c>
       <c r="W16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($H$7:W$7)+$I$4))),TREND($D16:$E16,$D$7:$E$7,W$7))</f>
-        <v>0</v>
+        <v>2.0392156862744981E-2</v>
       </c>
       <c r="X16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($H$7:X$7)+$I$4))),TREND($D16:$E16,$D$7:$E$7,X$7))</f>
-        <v>0</v>
+        <v>2.0007399186089514E-2</v>
       </c>
       <c r="Y16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($H$7:Y$7)+$I$4))),TREND($D16:$E16,$D$7:$E$7,Y$7))</f>
-        <v>0</v>
+        <v>1.9622641509433936E-2</v>
       </c>
       <c r="Z16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($H$7:Z$7)+$I$4))),TREND($D16:$E16,$D$7:$E$7,Z$7))</f>
-        <v>0</v>
+        <v>1.9237883832778357E-2</v>
       </c>
       <c r="AA16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($H$7:AA$7)+$I$4))),TREND($D16:$E16,$D$7:$E$7,AA$7))</f>
-        <v>0</v>
+        <v>1.8853126156122779E-2</v>
       </c>
       <c r="AB16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($H$7:AB$7)+$I$4))),TREND($D16:$E16,$D$7:$E$7,AB$7))</f>
-        <v>0</v>
+        <v>1.8468368479467201E-2</v>
       </c>
       <c r="AC16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($H$7:AC$7)+$I$4))),TREND($D16:$E16,$D$7:$E$7,AC$7))</f>
-        <v>0</v>
+        <v>1.8083610802811623E-2</v>
       </c>
       <c r="AD16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($H$7:AD$7)+$I$4))),TREND($D16:$E16,$D$7:$E$7,AD$7))</f>
-        <v>0</v>
+        <v>1.7698853126156044E-2</v>
       </c>
       <c r="AE16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($H$7:AE$7)+$I$4))),TREND($D16:$E16,$D$7:$E$7,AE$7))</f>
-        <v>0</v>
+        <v>1.7314095449500466E-2</v>
       </c>
       <c r="AF16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($H$7:AF$7)+$I$4))),TREND($D16:$E16,$D$7:$E$7,AF$7))</f>
-        <v>0</v>
+        <v>1.6929337772844888E-2</v>
       </c>
       <c r="AG16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($H$7:AG$7)+$I$4))),TREND($D16:$E16,$D$7:$E$7,AG$7))</f>
-        <v>0</v>
+        <v>1.654458009618931E-2</v>
       </c>
       <c r="AH16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($H$7:AH$7)+$I$4))),TREND($D16:$E16,$D$7:$E$7,AH$7))</f>
-        <v>0</v>
+        <v>1.6159822419533731E-2</v>
       </c>
       <c r="AI16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($H$7:AI$7)+$I$4))),TREND($D16:$E16,$D$7:$E$7,AI$7))</f>
-        <v>0</v>
+        <v>1.5775064742878264E-2</v>
       </c>
       <c r="AJ16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($H$7:AJ$7)+$I$4))),TREND($D16:$E16,$D$7:$E$7,AJ$7))</f>
-        <v>0</v>
+        <v>1.5390307066222686E-2</v>
       </c>
       <c r="AK16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($H$7:AK$7)+$I$4))),TREND($D16:$E16,$D$7:$E$7,AK$7))</f>
-        <v>0</v>
+        <v>1.5005549389567108E-2</v>
       </c>
       <c r="AL16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($H$7:AL$7)+$I$4))),TREND($D16:$E16,$D$7:$E$7,AL$7))</f>
-        <v>0</v>
+        <v>1.4620791712911529E-2</v>
       </c>
       <c r="AM16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($H$7:AM$7)+$I$4))),TREND($D16:$E16,$D$7:$E$7,AM$7))</f>
-        <v>0</v>
+        <v>1.4236034036255951E-2</v>
       </c>
       <c r="AN16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($H$7:AN$7)+$I$4))),TREND($D16:$E16,$D$7:$E$7,AN$7))</f>
-        <v>0</v>
+        <v>1.3851276359600373E-2</v>
       </c>
       <c r="AO16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($H$7:AO$7)+$I$4))),TREND($D16:$E16,$D$7:$E$7,AO$7))</f>
-        <v>0</v>
+        <v>1.3466518682944795E-2</v>
       </c>
       <c r="AP16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($H$7:AP$7)+$I$4))),TREND($D16:$E16,$D$7:$E$7,AP$7))</f>
-        <v>0</v>
+        <v>1.3081761006289216E-2</v>
       </c>
     </row>
     <row r="17" spans="1:42" x14ac:dyDescent="0.45">
@@ -13707,12 +13705,11 @@
         <v>0</v>
       </c>
       <c r="E19" s="10">
-        <f>E15*'India Assumptions'!$A$36</f>
-        <v>7.4999999999999997E-2</v>
+        <v>0</v>
       </c>
       <c r="F19" s="15" t="str">
         <f t="shared" si="4"/>
-        <v>s-curve</v>
+        <v>n/a</v>
       </c>
       <c r="H19" s="10">
         <f t="shared" si="3"/>
@@ -13720,139 +13717,139 @@
       </c>
       <c r="I19">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($H$7:I$7)+$I$4))),TREND($D19:$E19,$D$7:$E$7,I$7))</f>
-        <v>1.488022930055813E-3</v>
+        <v>0</v>
       </c>
       <c r="J19">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($H$7:J$7)+$I$4))),TREND($D19:$E19,$D$7:$E$7,J$7))</f>
-        <v>1.9947745182649396E-3</v>
+        <v>0</v>
       </c>
       <c r="K19">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($H$7:K$7)+$I$4))),TREND($D19:$E19,$D$7:$E$7,K$7))</f>
-        <v>2.6678391954477131E-3</v>
+        <v>0</v>
       </c>
       <c r="L19">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($H$7:L$7)+$I$4))),TREND($D19:$E19,$D$7:$E$7,L$7))</f>
-        <v>3.5569404883175086E-3</v>
+        <v>0</v>
       </c>
       <c r="M19">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($H$7:M$7)+$I$4))),TREND($D19:$E19,$D$7:$E$7,M$7))</f>
-        <v>4.7230017042747376E-3</v>
+        <v>0</v>
       </c>
       <c r="N19">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($H$7:N$7)+$I$4))),TREND($D19:$E19,$D$7:$E$7,N$7))</f>
-        <v>6.2379522370441774E-3</v>
+        <v>0</v>
       </c>
       <c r="O19">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($H$7:O$7)+$I$4))),TREND($D19:$E19,$D$7:$E$7,O$7))</f>
-        <v>8.182261589670968E-3</v>
+        <v>0</v>
       </c>
       <c r="P19">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($H$7:P$7)+$I$4))),TREND($D19:$E19,$D$7:$E$7,P$7))</f>
-        <v>1.0638829867536587E-2</v>
+        <v>0</v>
       </c>
       <c r="Q19">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($H$7:Q$7)+$I$4))),TREND($D19:$E19,$D$7:$E$7,Q$7))</f>
-        <v>1.3681914285476725E-2</v>
+        <v>0</v>
       </c>
       <c r="R19">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($H$7:R$7)+$I$4))),TREND($D19:$E19,$D$7:$E$7,R$7))</f>
-        <v>1.7360641237573676E-2</v>
+        <v>0</v>
       </c>
       <c r="S19">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($H$7:S$7)+$I$4))),TREND($D19:$E19,$D$7:$E$7,S$7))</f>
-        <v>2.1678787303124704E-2</v>
+        <v>0</v>
       </c>
       <c r="T19">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($H$7:T$7)+$I$4))),TREND($D19:$E19,$D$7:$E$7,T$7))</f>
-        <v>2.657577703306534E-2</v>
+        <v>0</v>
       </c>
       <c r="U19">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($H$7:U$7)+$I$4))),TREND($D19:$E19,$D$7:$E$7,U$7))</f>
-        <v>3.1916811239125577E-2</v>
+        <v>0</v>
       </c>
       <c r="V19">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($H$7:V$7)+$I$4))),TREND($D19:$E19,$D$7:$E$7,V$7))</f>
-        <v>3.7499999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="W19">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($H$7:W$7)+$I$4))),TREND($D19:$E19,$D$7:$E$7,W$7))</f>
-        <v>4.3083188760874427E-2</v>
+        <v>0</v>
       </c>
       <c r="X19">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($H$7:X$7)+$I$4))),TREND($D19:$E19,$D$7:$E$7,X$7))</f>
-        <v>4.8424222966934653E-2</v>
+        <v>0</v>
       </c>
       <c r="Y19">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($H$7:Y$7)+$I$4))),TREND($D19:$E19,$D$7:$E$7,Y$7))</f>
-        <v>5.3321212696875293E-2</v>
+        <v>0</v>
       </c>
       <c r="Z19">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($H$7:Z$7)+$I$4))),TREND($D19:$E19,$D$7:$E$7,Z$7))</f>
-        <v>5.7639358762426318E-2</v>
+        <v>0</v>
       </c>
       <c r="AA19">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($H$7:AA$7)+$I$4))),TREND($D19:$E19,$D$7:$E$7,AA$7))</f>
-        <v>6.1318085714523268E-2</v>
+        <v>0</v>
       </c>
       <c r="AB19">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($H$7:AB$7)+$I$4))),TREND($D19:$E19,$D$7:$E$7,AB$7))</f>
-        <v>6.4361170132463424E-2</v>
+        <v>0</v>
       </c>
       <c r="AC19">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($H$7:AC$7)+$I$4))),TREND($D19:$E19,$D$7:$E$7,AC$7))</f>
-        <v>6.6817738410329036E-2</v>
+        <v>0</v>
       </c>
       <c r="AD19">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($H$7:AD$7)+$I$4))),TREND($D19:$E19,$D$7:$E$7,AD$7))</f>
-        <v>6.8762047762955816E-2</v>
+        <v>0</v>
       </c>
       <c r="AE19">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($H$7:AE$7)+$I$4))),TREND($D19:$E19,$D$7:$E$7,AE$7))</f>
-        <v>7.0276998295725257E-2</v>
+        <v>0</v>
       </c>
       <c r="AF19">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($H$7:AF$7)+$I$4))),TREND($D19:$E19,$D$7:$E$7,AF$7))</f>
-        <v>7.1443059511682491E-2</v>
+        <v>0</v>
       </c>
       <c r="AG19">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($H$7:AG$7)+$I$4))),TREND($D19:$E19,$D$7:$E$7,AG$7))</f>
-        <v>7.2332160804552292E-2</v>
+        <v>0</v>
       </c>
       <c r="AH19">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($H$7:AH$7)+$I$4))),TREND($D19:$E19,$D$7:$E$7,AH$7))</f>
-        <v>7.3005225481735048E-2</v>
+        <v>0</v>
       </c>
       <c r="AI19">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($H$7:AI$7)+$I$4))),TREND($D19:$E19,$D$7:$E$7,AI$7))</f>
-        <v>7.3511977069944182E-2</v>
+        <v>0</v>
       </c>
       <c r="AJ19">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($H$7:AJ$7)+$I$4))),TREND($D19:$E19,$D$7:$E$7,AJ$7))</f>
-        <v>7.3891947623004522E-2</v>
+        <v>0</v>
       </c>
       <c r="AK19">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($H$7:AK$7)+$I$4))),TREND($D19:$E19,$D$7:$E$7,AK$7))</f>
-        <v>7.4175979302705516E-2</v>
+        <v>0</v>
       </c>
       <c r="AL19">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($H$7:AL$7)+$I$4))),TREND($D19:$E19,$D$7:$E$7,AL$7))</f>
-        <v>7.4387807163513009E-2</v>
+        <v>0</v>
       </c>
       <c r="AM19">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($H$7:AM$7)+$I$4))),TREND($D19:$E19,$D$7:$E$7,AM$7))</f>
-        <v>7.4545514888131187E-2</v>
+        <v>0</v>
       </c>
       <c r="AN19">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($H$7:AN$7)+$I$4))),TREND($D19:$E19,$D$7:$E$7,AN$7))</f>
-        <v>7.4662779512929406E-2</v>
+        <v>0</v>
       </c>
       <c r="AO19">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($H$7:AO$7)+$I$4))),TREND($D19:$E19,$D$7:$E$7,AO$7))</f>
-        <v>7.4749889451943996E-2</v>
+        <v>0</v>
       </c>
       <c r="AP19">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($H$7:AP$7)+$I$4))),TREND($D19:$E19,$D$7:$E$7,AP$7))</f>
-        <v>7.4814553263252398E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:42" x14ac:dyDescent="0.45">
@@ -14815,12 +14812,11 @@
         <v>0</v>
       </c>
       <c r="E26" s="10">
-        <f>E22*'India Assumptions'!$A$36</f>
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="F26" s="15" t="str">
         <f t="shared" si="4"/>
-        <v>s-curve</v>
+        <v>n/a</v>
       </c>
       <c r="H26" s="10">
         <f t="shared" si="3"/>
@@ -14828,139 +14824,139 @@
       </c>
       <c r="I26">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($H$7:I$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,I$7))</f>
-        <v>5.9520917202232522E-3</v>
+        <v>0</v>
       </c>
       <c r="J26">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($H$7:J$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,J$7))</f>
-        <v>7.9790980730597583E-3</v>
+        <v>0</v>
       </c>
       <c r="K26">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($H$7:K$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,K$7))</f>
-        <v>1.0671356781790852E-2</v>
+        <v>0</v>
       </c>
       <c r="L26">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($H$7:L$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,L$7))</f>
-        <v>1.4227761953270034E-2</v>
+        <v>0</v>
       </c>
       <c r="M26">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($H$7:M$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,M$7))</f>
-        <v>1.889200681709895E-2</v>
+        <v>0</v>
       </c>
       <c r="N26">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($H$7:N$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,N$7))</f>
-        <v>2.495180894817671E-2</v>
+        <v>0</v>
       </c>
       <c r="O26">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($H$7:O$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,O$7))</f>
-        <v>3.2729046358683872E-2</v>
+        <v>0</v>
       </c>
       <c r="P26">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($H$7:P$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,P$7))</f>
-        <v>4.2555319470146347E-2</v>
+        <v>0</v>
       </c>
       <c r="Q26">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($H$7:Q$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,Q$7))</f>
-        <v>5.4727657141906902E-2</v>
+        <v>0</v>
       </c>
       <c r="R26">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($H$7:R$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,R$7))</f>
-        <v>6.9442564950294702E-2</v>
+        <v>0</v>
       </c>
       <c r="S26">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($H$7:S$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,S$7))</f>
-        <v>8.6715149212498815E-2</v>
+        <v>0</v>
       </c>
       <c r="T26">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($H$7:T$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,T$7))</f>
-        <v>0.10630310813226136</v>
+        <v>0</v>
       </c>
       <c r="U26">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($H$7:U$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,U$7))</f>
-        <v>0.12766724495650231</v>
+        <v>0</v>
       </c>
       <c r="V26">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($H$7:V$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,V$7))</f>
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="W26">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($H$7:W$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,W$7))</f>
-        <v>0.17233275504349771</v>
+        <v>0</v>
       </c>
       <c r="X26">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($H$7:X$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,X$7))</f>
-        <v>0.19369689186773861</v>
+        <v>0</v>
       </c>
       <c r="Y26">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($H$7:Y$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,Y$7))</f>
-        <v>0.21328485078750117</v>
+        <v>0</v>
       </c>
       <c r="Z26">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($H$7:Z$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,Z$7))</f>
-        <v>0.23055743504970527</v>
+        <v>0</v>
       </c>
       <c r="AA26">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($H$7:AA$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,AA$7))</f>
-        <v>0.24527234285809307</v>
+        <v>0</v>
       </c>
       <c r="AB26">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($H$7:AB$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,AB$7))</f>
-        <v>0.2574446805298537</v>
+        <v>0</v>
       </c>
       <c r="AC26">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($H$7:AC$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,AC$7))</f>
-        <v>0.26727095364131614</v>
+        <v>0</v>
       </c>
       <c r="AD26">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($H$7:AD$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,AD$7))</f>
-        <v>0.27504819105182327</v>
+        <v>0</v>
       </c>
       <c r="AE26">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($H$7:AE$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,AE$7))</f>
-        <v>0.28110799318290103</v>
+        <v>0</v>
       </c>
       <c r="AF26">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($H$7:AF$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,AF$7))</f>
-        <v>0.28577223804672996</v>
+        <v>0</v>
       </c>
       <c r="AG26">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($H$7:AG$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,AG$7))</f>
-        <v>0.28932864321820917</v>
+        <v>0</v>
       </c>
       <c r="AH26">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($H$7:AH$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,AH$7))</f>
-        <v>0.29202090192694019</v>
+        <v>0</v>
       </c>
       <c r="AI26">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($H$7:AI$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,AI$7))</f>
-        <v>0.29404790827977673</v>
+        <v>0</v>
       </c>
       <c r="AJ26">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($H$7:AJ$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,AJ$7))</f>
-        <v>0.29556779049201809</v>
+        <v>0</v>
       </c>
       <c r="AK26">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($H$7:AK$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,AK$7))</f>
-        <v>0.29670391721082207</v>
+        <v>0</v>
       </c>
       <c r="AL26">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($H$7:AL$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,AL$7))</f>
-        <v>0.29755122865405204</v>
+        <v>0</v>
       </c>
       <c r="AM26">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($H$7:AM$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,AM$7))</f>
-        <v>0.29818205955252475</v>
+        <v>0</v>
       </c>
       <c r="AN26">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($H$7:AN$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,AN$7))</f>
-        <v>0.29865111805171762</v>
+        <v>0</v>
       </c>
       <c r="AO26">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($H$7:AO$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,AO$7))</f>
-        <v>0.29899955780777598</v>
+        <v>0</v>
       </c>
       <c r="AP26">
         <f>IF($F26="s-curve",$D26+($E26-$D26)*$I$2/(1+EXP($I$3*(COUNT($H$7:AP$7)+$I$4))),TREND($D26:$E26,$D$7:$E$7,AP$7))</f>
-        <v>0.29925821305300959</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:42" x14ac:dyDescent="0.45">
@@ -15294,7 +15290,6 @@
         <v>0</v>
       </c>
       <c r="E29" s="10">
-        <f>E22*'India Assumptions'!$A$31</f>
         <v>0.15</v>
       </c>
       <c r="F29" s="15" t="str">
@@ -15922,12 +15917,11 @@
         <v>0</v>
       </c>
       <c r="E33" s="10">
-        <f>E29*'India Assumptions'!$A$36</f>
-        <v>7.4999999999999997E-2</v>
+        <v>0</v>
       </c>
       <c r="F33" s="15" t="str">
         <f t="shared" si="4"/>
-        <v>s-curve</v>
+        <v>n/a</v>
       </c>
       <c r="H33" s="10">
         <f t="shared" si="3"/>
@@ -15935,139 +15929,139 @@
       </c>
       <c r="I33">
         <f>IF($F33="s-curve",$D33+($E33-$D33)*$I$2/(1+EXP($I$3*(COUNT($H$7:I$7)+$I$4))),TREND($D33:$E33,$D$7:$E$7,I$7))</f>
-        <v>1.488022930055813E-3</v>
+        <v>0</v>
       </c>
       <c r="J33">
         <f>IF($F33="s-curve",$D33+($E33-$D33)*$I$2/(1+EXP($I$3*(COUNT($H$7:J$7)+$I$4))),TREND($D33:$E33,$D$7:$E$7,J$7))</f>
-        <v>1.9947745182649396E-3</v>
+        <v>0</v>
       </c>
       <c r="K33">
         <f>IF($F33="s-curve",$D33+($E33-$D33)*$I$2/(1+EXP($I$3*(COUNT($H$7:K$7)+$I$4))),TREND($D33:$E33,$D$7:$E$7,K$7))</f>
-        <v>2.6678391954477131E-3</v>
+        <v>0</v>
       </c>
       <c r="L33">
         <f>IF($F33="s-curve",$D33+($E33-$D33)*$I$2/(1+EXP($I$3*(COUNT($H$7:L$7)+$I$4))),TREND($D33:$E33,$D$7:$E$7,L$7))</f>
-        <v>3.5569404883175086E-3</v>
+        <v>0</v>
       </c>
       <c r="M33">
         <f>IF($F33="s-curve",$D33+($E33-$D33)*$I$2/(1+EXP($I$3*(COUNT($H$7:M$7)+$I$4))),TREND($D33:$E33,$D$7:$E$7,M$7))</f>
-        <v>4.7230017042747376E-3</v>
+        <v>0</v>
       </c>
       <c r="N33">
         <f>IF($F33="s-curve",$D33+($E33-$D33)*$I$2/(1+EXP($I$3*(COUNT($H$7:N$7)+$I$4))),TREND($D33:$E33,$D$7:$E$7,N$7))</f>
-        <v>6.2379522370441774E-3</v>
+        <v>0</v>
       </c>
       <c r="O33">
         <f>IF($F33="s-curve",$D33+($E33-$D33)*$I$2/(1+EXP($I$3*(COUNT($H$7:O$7)+$I$4))),TREND($D33:$E33,$D$7:$E$7,O$7))</f>
-        <v>8.182261589670968E-3</v>
+        <v>0</v>
       </c>
       <c r="P33">
         <f>IF($F33="s-curve",$D33+($E33-$D33)*$I$2/(1+EXP($I$3*(COUNT($H$7:P$7)+$I$4))),TREND($D33:$E33,$D$7:$E$7,P$7))</f>
-        <v>1.0638829867536587E-2</v>
+        <v>0</v>
       </c>
       <c r="Q33">
         <f>IF($F33="s-curve",$D33+($E33-$D33)*$I$2/(1+EXP($I$3*(COUNT($H$7:Q$7)+$I$4))),TREND($D33:$E33,$D$7:$E$7,Q$7))</f>
-        <v>1.3681914285476725E-2</v>
+        <v>0</v>
       </c>
       <c r="R33">
         <f>IF($F33="s-curve",$D33+($E33-$D33)*$I$2/(1+EXP($I$3*(COUNT($H$7:R$7)+$I$4))),TREND($D33:$E33,$D$7:$E$7,R$7))</f>
-        <v>1.7360641237573676E-2</v>
+        <v>0</v>
       </c>
       <c r="S33">
         <f>IF($F33="s-curve",$D33+($E33-$D33)*$I$2/(1+EXP($I$3*(COUNT($H$7:S$7)+$I$4))),TREND($D33:$E33,$D$7:$E$7,S$7))</f>
-        <v>2.1678787303124704E-2</v>
+        <v>0</v>
       </c>
       <c r="T33">
         <f>IF($F33="s-curve",$D33+($E33-$D33)*$I$2/(1+EXP($I$3*(COUNT($H$7:T$7)+$I$4))),TREND($D33:$E33,$D$7:$E$7,T$7))</f>
-        <v>2.657577703306534E-2</v>
+        <v>0</v>
       </c>
       <c r="U33">
         <f>IF($F33="s-curve",$D33+($E33-$D33)*$I$2/(1+EXP($I$3*(COUNT($H$7:U$7)+$I$4))),TREND($D33:$E33,$D$7:$E$7,U$7))</f>
-        <v>3.1916811239125577E-2</v>
+        <v>0</v>
       </c>
       <c r="V33">
         <f>IF($F33="s-curve",$D33+($E33-$D33)*$I$2/(1+EXP($I$3*(COUNT($H$7:V$7)+$I$4))),TREND($D33:$E33,$D$7:$E$7,V$7))</f>
-        <v>3.7499999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="W33">
         <f>IF($F33="s-curve",$D33+($E33-$D33)*$I$2/(1+EXP($I$3*(COUNT($H$7:W$7)+$I$4))),TREND($D33:$E33,$D$7:$E$7,W$7))</f>
-        <v>4.3083188760874427E-2</v>
+        <v>0</v>
       </c>
       <c r="X33">
         <f>IF($F33="s-curve",$D33+($E33-$D33)*$I$2/(1+EXP($I$3*(COUNT($H$7:X$7)+$I$4))),TREND($D33:$E33,$D$7:$E$7,X$7))</f>
-        <v>4.8424222966934653E-2</v>
+        <v>0</v>
       </c>
       <c r="Y33">
         <f>IF($F33="s-curve",$D33+($E33-$D33)*$I$2/(1+EXP($I$3*(COUNT($H$7:Y$7)+$I$4))),TREND($D33:$E33,$D$7:$E$7,Y$7))</f>
-        <v>5.3321212696875293E-2</v>
+        <v>0</v>
       </c>
       <c r="Z33">
         <f>IF($F33="s-curve",$D33+($E33-$D33)*$I$2/(1+EXP($I$3*(COUNT($H$7:Z$7)+$I$4))),TREND($D33:$E33,$D$7:$E$7,Z$7))</f>
-        <v>5.7639358762426318E-2</v>
+        <v>0</v>
       </c>
       <c r="AA33">
         <f>IF($F33="s-curve",$D33+($E33-$D33)*$I$2/(1+EXP($I$3*(COUNT($H$7:AA$7)+$I$4))),TREND($D33:$E33,$D$7:$E$7,AA$7))</f>
-        <v>6.1318085714523268E-2</v>
+        <v>0</v>
       </c>
       <c r="AB33">
         <f>IF($F33="s-curve",$D33+($E33-$D33)*$I$2/(1+EXP($I$3*(COUNT($H$7:AB$7)+$I$4))),TREND($D33:$E33,$D$7:$E$7,AB$7))</f>
-        <v>6.4361170132463424E-2</v>
+        <v>0</v>
       </c>
       <c r="AC33">
         <f>IF($F33="s-curve",$D33+($E33-$D33)*$I$2/(1+EXP($I$3*(COUNT($H$7:AC$7)+$I$4))),TREND($D33:$E33,$D$7:$E$7,AC$7))</f>
-        <v>6.6817738410329036E-2</v>
+        <v>0</v>
       </c>
       <c r="AD33">
         <f>IF($F33="s-curve",$D33+($E33-$D33)*$I$2/(1+EXP($I$3*(COUNT($H$7:AD$7)+$I$4))),TREND($D33:$E33,$D$7:$E$7,AD$7))</f>
-        <v>6.8762047762955816E-2</v>
+        <v>0</v>
       </c>
       <c r="AE33">
         <f>IF($F33="s-curve",$D33+($E33-$D33)*$I$2/(1+EXP($I$3*(COUNT($H$7:AE$7)+$I$4))),TREND($D33:$E33,$D$7:$E$7,AE$7))</f>
-        <v>7.0276998295725257E-2</v>
+        <v>0</v>
       </c>
       <c r="AF33">
         <f>IF($F33="s-curve",$D33+($E33-$D33)*$I$2/(1+EXP($I$3*(COUNT($H$7:AF$7)+$I$4))),TREND($D33:$E33,$D$7:$E$7,AF$7))</f>
-        <v>7.1443059511682491E-2</v>
+        <v>0</v>
       </c>
       <c r="AG33">
         <f>IF($F33="s-curve",$D33+($E33-$D33)*$I$2/(1+EXP($I$3*(COUNT($H$7:AG$7)+$I$4))),TREND($D33:$E33,$D$7:$E$7,AG$7))</f>
-        <v>7.2332160804552292E-2</v>
+        <v>0</v>
       </c>
       <c r="AH33">
         <f>IF($F33="s-curve",$D33+($E33-$D33)*$I$2/(1+EXP($I$3*(COUNT($H$7:AH$7)+$I$4))),TREND($D33:$E33,$D$7:$E$7,AH$7))</f>
-        <v>7.3005225481735048E-2</v>
+        <v>0</v>
       </c>
       <c r="AI33">
         <f>IF($F33="s-curve",$D33+($E33-$D33)*$I$2/(1+EXP($I$3*(COUNT($H$7:AI$7)+$I$4))),TREND($D33:$E33,$D$7:$E$7,AI$7))</f>
-        <v>7.3511977069944182E-2</v>
+        <v>0</v>
       </c>
       <c r="AJ33">
         <f>IF($F33="s-curve",$D33+($E33-$D33)*$I$2/(1+EXP($I$3*(COUNT($H$7:AJ$7)+$I$4))),TREND($D33:$E33,$D$7:$E$7,AJ$7))</f>
-        <v>7.3891947623004522E-2</v>
+        <v>0</v>
       </c>
       <c r="AK33">
         <f>IF($F33="s-curve",$D33+($E33-$D33)*$I$2/(1+EXP($I$3*(COUNT($H$7:AK$7)+$I$4))),TREND($D33:$E33,$D$7:$E$7,AK$7))</f>
-        <v>7.4175979302705516E-2</v>
+        <v>0</v>
       </c>
       <c r="AL33">
         <f>IF($F33="s-curve",$D33+($E33-$D33)*$I$2/(1+EXP($I$3*(COUNT($H$7:AL$7)+$I$4))),TREND($D33:$E33,$D$7:$E$7,AL$7))</f>
-        <v>7.4387807163513009E-2</v>
+        <v>0</v>
       </c>
       <c r="AM33">
         <f>IF($F33="s-curve",$D33+($E33-$D33)*$I$2/(1+EXP($I$3*(COUNT($H$7:AM$7)+$I$4))),TREND($D33:$E33,$D$7:$E$7,AM$7))</f>
-        <v>7.4545514888131187E-2</v>
+        <v>0</v>
       </c>
       <c r="AN33">
         <f>IF($F33="s-curve",$D33+($E33-$D33)*$I$2/(1+EXP($I$3*(COUNT($H$7:AN$7)+$I$4))),TREND($D33:$E33,$D$7:$E$7,AN$7))</f>
-        <v>7.4662779512929406E-2</v>
+        <v>0</v>
       </c>
       <c r="AO33">
         <f>IF($F33="s-curve",$D33+($E33-$D33)*$I$2/(1+EXP($I$3*(COUNT($H$7:AO$7)+$I$4))),TREND($D33:$E33,$D$7:$E$7,AO$7))</f>
-        <v>7.4749889451943996E-2</v>
+        <v>0</v>
       </c>
       <c r="AP33">
         <f>IF($F33="s-curve",$D33+($E33-$D33)*$I$2/(1+EXP($I$3*(COUNT($H$7:AP$7)+$I$4))),TREND($D33:$E33,$D$7:$E$7,AP$7))</f>
-        <v>7.4814553263252398E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:42" x14ac:dyDescent="0.45">
@@ -24099,8 +24093,7 @@
         <v>3.3749999999999995E-2</v>
       </c>
       <c r="E85" s="10">
-        <f>E78*'India Assumptions'!$A$31</f>
-        <v>0.15</v>
+        <v>0.3</v>
       </c>
       <c r="F85" s="15" t="str">
         <f t="shared" ref="F85:F91" si="10">IF(D85=E85,"n/a",IF(OR(C85="battery electric vehicle",C85="plugin hybrid vehicle"),"s-curve","linear"))</f>
@@ -24112,139 +24105,139 @@
       </c>
       <c r="I85">
         <f>IF($F85="s-curve",$D85+($E85-$D85)*$I$2/(1+EXP($I$3*(COUNT($H$7:I$7)+$I$4))),TREND($D85:$E85,$D$7:$E$7,I$7))</f>
-        <v>3.6056435541586503E-2</v>
+        <v>3.9032481401698134E-2</v>
       </c>
       <c r="J85">
         <f>IF($F85="s-curve",$D85+($E85-$D85)*$I$2/(1+EXP($I$3*(COUNT($H$7:J$7)+$I$4))),TREND($D85:$E85,$D$7:$E$7,J$7))</f>
-        <v>3.6841900503310654E-2</v>
+        <v>4.0831449539840532E-2</v>
       </c>
       <c r="K85">
         <f>IF($F85="s-curve",$D85+($E85-$D85)*$I$2/(1+EXP($I$3*(COUNT($H$7:K$7)+$I$4))),TREND($D85:$E85,$D$7:$E$7,K$7))</f>
-        <v>3.788515075294395E-2</v>
+        <v>4.3220829143839373E-2</v>
       </c>
       <c r="L85">
         <f>IF($F85="s-curve",$D85+($E85-$D85)*$I$2/(1+EXP($I$3*(COUNT($H$7:L$7)+$I$4))),TREND($D85:$E85,$D$7:$E$7,L$7))</f>
-        <v>3.9263257756892135E-2</v>
+        <v>4.6377138733527154E-2</v>
       </c>
       <c r="M85">
         <f>IF($F85="s-curve",$D85+($E85-$D85)*$I$2/(1+EXP($I$3*(COUNT($H$7:M$7)+$I$4))),TREND($D85:$E85,$D$7:$E$7,M$7))</f>
-        <v>4.1070652641625835E-2</v>
+        <v>5.0516656050175315E-2</v>
       </c>
       <c r="N85">
         <f>IF($F85="s-curve",$D85+($E85-$D85)*$I$2/(1+EXP($I$3*(COUNT($H$7:N$7)+$I$4))),TREND($D85:$E85,$D$7:$E$7,N$7))</f>
-        <v>4.3418825967418473E-2</v>
+        <v>5.5894730441506828E-2</v>
       </c>
       <c r="O85">
         <f>IF($F85="s-curve",$D85+($E85-$D85)*$I$2/(1+EXP($I$3*(COUNT($H$7:O$7)+$I$4))),TREND($D85:$E85,$D$7:$E$7,O$7))</f>
-        <v>4.6432505463989998E-2</v>
+        <v>6.2797028643331934E-2</v>
       </c>
       <c r="P85">
         <f>IF($F85="s-curve",$D85+($E85-$D85)*$I$2/(1+EXP($I$3*(COUNT($H$7:P$7)+$I$4))),TREND($D85:$E85,$D$7:$E$7,P$7))</f>
-        <v>5.0240186294681702E-2</v>
+        <v>7.1517846029754875E-2</v>
       </c>
       <c r="Q85">
         <f>IF($F85="s-curve",$D85+($E85-$D85)*$I$2/(1+EXP($I$3*(COUNT($H$7:Q$7)+$I$4))),TREND($D85:$E85,$D$7:$E$7,Q$7))</f>
-        <v>5.4956967142488919E-2</v>
+        <v>8.2320795713442363E-2</v>
       </c>
       <c r="R85">
         <f>IF($F85="s-curve",$D85+($E85-$D85)*$I$2/(1+EXP($I$3*(COUNT($H$7:R$7)+$I$4))),TREND($D85:$E85,$D$7:$E$7,R$7))</f>
-        <v>6.0658993918239194E-2</v>
+        <v>9.5380276393386546E-2</v>
       </c>
       <c r="S85">
         <f>IF($F85="s-curve",$D85+($E85-$D85)*$I$2/(1+EXP($I$3*(COUNT($H$7:S$7)+$I$4))),TREND($D85:$E85,$D$7:$E$7,S$7))</f>
-        <v>6.7352120319843278E-2</v>
+        <v>0.1107096949260927</v>
       </c>
       <c r="T85">
         <f>IF($F85="s-curve",$D85+($E85-$D85)*$I$2/(1+EXP($I$3*(COUNT($H$7:T$7)+$I$4))),TREND($D85:$E85,$D$7:$E$7,T$7))</f>
-        <v>7.4942454401251274E-2</v>
+        <v>0.12809400846738195</v>
       </c>
       <c r="U85">
         <f>IF($F85="s-curve",$D85+($E85-$D85)*$I$2/(1+EXP($I$3*(COUNT($H$7:U$7)+$I$4))),TREND($D85:$E85,$D$7:$E$7,U$7))</f>
-        <v>8.3221057420644631E-2</v>
+        <v>0.14705467989889578</v>
       </c>
       <c r="V85">
         <f>IF($F85="s-curve",$D85+($E85-$D85)*$I$2/(1+EXP($I$3*(COUNT($H$7:V$7)+$I$4))),TREND($D85:$E85,$D$7:$E$7,V$7))</f>
-        <v>9.1874999999999984E-2</v>
+        <v>0.166875</v>
       </c>
       <c r="W85">
         <f>IF($F85="s-curve",$D85+($E85-$D85)*$I$2/(1+EXP($I$3*(COUNT($H$7:W$7)+$I$4))),TREND($D85:$E85,$D$7:$E$7,W$7))</f>
-        <v>0.10052894257935535</v>
+        <v>0.18669532010110421</v>
       </c>
       <c r="X85">
         <f>IF($F85="s-curve",$D85+($E85-$D85)*$I$2/(1+EXP($I$3*(COUNT($H$7:X$7)+$I$4))),TREND($D85:$E85,$D$7:$E$7,X$7))</f>
-        <v>0.1088075455987487</v>
+        <v>0.20565599153261802</v>
       </c>
       <c r="Y85">
         <f>IF($F85="s-curve",$D85+($E85-$D85)*$I$2/(1+EXP($I$3*(COUNT($H$7:Y$7)+$I$4))),TREND($D85:$E85,$D$7:$E$7,Y$7))</f>
-        <v>0.11639787968015669</v>
+        <v>0.22304030507390729</v>
       </c>
       <c r="Z85">
         <f>IF($F85="s-curve",$D85+($E85-$D85)*$I$2/(1+EXP($I$3*(COUNT($H$7:Z$7)+$I$4))),TREND($D85:$E85,$D$7:$E$7,Z$7))</f>
-        <v>0.1230910060817608</v>
+        <v>0.23836972360661343</v>
       </c>
       <c r="AA85">
         <f>IF($F85="s-curve",$D85+($E85-$D85)*$I$2/(1+EXP($I$3*(COUNT($H$7:AA$7)+$I$4))),TREND($D85:$E85,$D$7:$E$7,AA$7))</f>
-        <v>0.12879303285751106</v>
+        <v>0.25142920428655757</v>
       </c>
       <c r="AB85">
         <f>IF($F85="s-curve",$D85+($E85-$D85)*$I$2/(1+EXP($I$3*(COUNT($H$7:AB$7)+$I$4))),TREND($D85:$E85,$D$7:$E$7,AB$7))</f>
-        <v>0.13350981370531828</v>
+        <v>0.26223215397024513</v>
       </c>
       <c r="AC85">
         <f>IF($F85="s-curve",$D85+($E85-$D85)*$I$2/(1+EXP($I$3*(COUNT($H$7:AC$7)+$I$4))),TREND($D85:$E85,$D$7:$E$7,AC$7))</f>
-        <v>0.13731749453601</v>
+        <v>0.27095297135666802</v>
       </c>
       <c r="AD85">
         <f>IF($F85="s-curve",$D85+($E85-$D85)*$I$2/(1+EXP($I$3*(COUNT($H$7:AD$7)+$I$4))),TREND($D85:$E85,$D$7:$E$7,AD$7))</f>
-        <v>0.14033117403258152</v>
+        <v>0.27785526955849316</v>
       </c>
       <c r="AE85">
         <f>IF($F85="s-curve",$D85+($E85-$D85)*$I$2/(1+EXP($I$3*(COUNT($H$7:AE$7)+$I$4))),TREND($D85:$E85,$D$7:$E$7,AE$7))</f>
-        <v>0.14267934735837415</v>
+        <v>0.28323334394982469</v>
       </c>
       <c r="AF85">
         <f>IF($F85="s-curve",$D85+($E85-$D85)*$I$2/(1+EXP($I$3*(COUNT($H$7:AF$7)+$I$4))),TREND($D85:$E85,$D$7:$E$7,AF$7))</f>
-        <v>0.14448674224310787</v>
+        <v>0.28737286126647288</v>
       </c>
       <c r="AG85">
         <f>IF($F85="s-curve",$D85+($E85-$D85)*$I$2/(1+EXP($I$3*(COUNT($H$7:AG$7)+$I$4))),TREND($D85:$E85,$D$7:$E$7,AG$7))</f>
-        <v>0.14586484924705603</v>
+        <v>0.29052917085616059</v>
       </c>
       <c r="AH85">
         <f>IF($F85="s-curve",$D85+($E85-$D85)*$I$2/(1+EXP($I$3*(COUNT($H$7:AH$7)+$I$4))),TREND($D85:$E85,$D$7:$E$7,AH$7))</f>
-        <v>0.14690809949668931</v>
+        <v>0.29291855046015941</v>
       </c>
       <c r="AI85">
         <f>IF($F85="s-curve",$D85+($E85-$D85)*$I$2/(1+EXP($I$3*(COUNT($H$7:AI$7)+$I$4))),TREND($D85:$E85,$D$7:$E$7,AI$7))</f>
-        <v>0.14769356445841347</v>
+        <v>0.29471751859830186</v>
       </c>
       <c r="AJ85">
         <f>IF($F85="s-curve",$D85+($E85-$D85)*$I$2/(1+EXP($I$3*(COUNT($H$7:AJ$7)+$I$4))),TREND($D85:$E85,$D$7:$E$7,AJ$7))</f>
-        <v>0.14828251881565699</v>
+        <v>0.29606641406166606</v>
       </c>
       <c r="AK85">
         <f>IF($F85="s-curve",$D85+($E85-$D85)*$I$2/(1+EXP($I$3*(COUNT($H$7:AK$7)+$I$4))),TREND($D85:$E85,$D$7:$E$7,AK$7))</f>
-        <v>0.14872276791919353</v>
+        <v>0.29707472652460454</v>
       </c>
       <c r="AL85">
         <f>IF($F85="s-curve",$D85+($E85-$D85)*$I$2/(1+EXP($I$3*(COUNT($H$7:AL$7)+$I$4))),TREND($D85:$E85,$D$7:$E$7,AL$7))</f>
-        <v>0.14905110110344516</v>
+        <v>0.29782671543047118</v>
       </c>
       <c r="AM85">
         <f>IF($F85="s-curve",$D85+($E85-$D85)*$I$2/(1+EXP($I$3*(COUNT($H$7:AM$7)+$I$4))),TREND($D85:$E85,$D$7:$E$7,AM$7))</f>
-        <v>0.14929554807660333</v>
+        <v>0.29838657785286571</v>
       </c>
       <c r="AN85">
         <f>IF($F85="s-curve",$D85+($E85-$D85)*$I$2/(1+EXP($I$3*(COUNT($H$7:AN$7)+$I$4))),TREND($D85:$E85,$D$7:$E$7,AN$7))</f>
-        <v>0.14947730824504057</v>
+        <v>0.29880286727089939</v>
       </c>
       <c r="AO85">
         <f>IF($F85="s-curve",$D85+($E85-$D85)*$I$2/(1+EXP($I$3*(COUNT($H$7:AO$7)+$I$4))),TREND($D85:$E85,$D$7:$E$7,AO$7))</f>
-        <v>0.14961232865051319</v>
+        <v>0.29911210755440121</v>
       </c>
       <c r="AP85">
         <f>IF($F85="s-curve",$D85+($E85-$D85)*$I$2/(1+EXP($I$3*(COUNT($H$7:AP$7)+$I$4))),TREND($D85:$E85,$D$7:$E$7,AP$7))</f>
-        <v>0.14971255755804119</v>
+        <v>0.29934166408454599</v>
       </c>
     </row>
     <row r="86" spans="1:42" x14ac:dyDescent="0.45">
@@ -24728,7 +24721,7 @@
       </c>
       <c r="E89" s="10">
         <f>E85*'India Assumptions'!$A$36</f>
-        <v>7.4999999999999997E-2</v>
+        <v>0.15</v>
       </c>
       <c r="F89" s="15" t="str">
         <f t="shared" si="10"/>
@@ -24740,139 +24733,139 @@
       </c>
       <c r="I89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:I$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,I$7))</f>
-        <v>1.488022930055813E-3</v>
+        <v>2.9760458601116261E-3</v>
       </c>
       <c r="J89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:J$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,J$7))</f>
-        <v>1.9947745182649396E-3</v>
+        <v>3.9895490365298792E-3</v>
       </c>
       <c r="K89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:K$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,K$7))</f>
-        <v>2.6678391954477131E-3</v>
+        <v>5.3356783908954262E-3</v>
       </c>
       <c r="L89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:L$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,L$7))</f>
-        <v>3.5569404883175086E-3</v>
+        <v>7.1138809766350172E-3</v>
       </c>
       <c r="M89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:M$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,M$7))</f>
-        <v>4.7230017042747376E-3</v>
+        <v>9.4460034085494752E-3</v>
       </c>
       <c r="N89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:N$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,N$7))</f>
-        <v>6.2379522370441774E-3</v>
+        <v>1.2475904474088355E-2</v>
       </c>
       <c r="O89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:O$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,O$7))</f>
-        <v>8.182261589670968E-3</v>
+        <v>1.6364523179341936E-2</v>
       </c>
       <c r="P89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:P$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,P$7))</f>
-        <v>1.0638829867536587E-2</v>
+        <v>2.1277659735073173E-2</v>
       </c>
       <c r="Q89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:Q$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,Q$7))</f>
-        <v>1.3681914285476725E-2</v>
+        <v>2.7363828570953451E-2</v>
       </c>
       <c r="R89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:R$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,R$7))</f>
-        <v>1.7360641237573676E-2</v>
+        <v>3.4721282475147351E-2</v>
       </c>
       <c r="S89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:S$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,S$7))</f>
-        <v>2.1678787303124704E-2</v>
+        <v>4.3357574606249408E-2</v>
       </c>
       <c r="T89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:T$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,T$7))</f>
-        <v>2.657577703306534E-2</v>
+        <v>5.3151554066130681E-2</v>
       </c>
       <c r="U89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:U$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,U$7))</f>
-        <v>3.1916811239125577E-2</v>
+        <v>6.3833622478251154E-2</v>
       </c>
       <c r="V89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:V$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,V$7))</f>
-        <v>3.7499999999999999E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="W89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:W$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,W$7))</f>
-        <v>4.3083188760874427E-2</v>
+        <v>8.6166377521748855E-2</v>
       </c>
       <c r="X89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:X$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,X$7))</f>
-        <v>4.8424222966934653E-2</v>
+        <v>9.6848445933869307E-2</v>
       </c>
       <c r="Y89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:Y$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,Y$7))</f>
-        <v>5.3321212696875293E-2</v>
+        <v>0.10664242539375059</v>
       </c>
       <c r="Z89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:Z$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,Z$7))</f>
-        <v>5.7639358762426318E-2</v>
+        <v>0.11527871752485264</v>
       </c>
       <c r="AA89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:AA$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,AA$7))</f>
-        <v>6.1318085714523268E-2</v>
+        <v>0.12263617142904654</v>
       </c>
       <c r="AB89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:AB$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,AB$7))</f>
-        <v>6.4361170132463424E-2</v>
+        <v>0.12872234026492685</v>
       </c>
       <c r="AC89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:AC$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,AC$7))</f>
-        <v>6.6817738410329036E-2</v>
+        <v>0.13363547682065807</v>
       </c>
       <c r="AD89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:AD$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,AD$7))</f>
-        <v>6.8762047762955816E-2</v>
+        <v>0.13752409552591163</v>
       </c>
       <c r="AE89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:AE$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,AE$7))</f>
-        <v>7.0276998295725257E-2</v>
+        <v>0.14055399659145051</v>
       </c>
       <c r="AF89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:AF$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,AF$7))</f>
-        <v>7.1443059511682491E-2</v>
+        <v>0.14288611902336498</v>
       </c>
       <c r="AG89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:AG$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,AG$7))</f>
-        <v>7.2332160804552292E-2</v>
+        <v>0.14466432160910458</v>
       </c>
       <c r="AH89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:AH$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,AH$7))</f>
-        <v>7.3005225481735048E-2</v>
+        <v>0.1460104509634701</v>
       </c>
       <c r="AI89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:AI$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,AI$7))</f>
-        <v>7.3511977069944182E-2</v>
+        <v>0.14702395413988836</v>
       </c>
       <c r="AJ89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:AJ$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,AJ$7))</f>
-        <v>7.3891947623004522E-2</v>
+        <v>0.14778389524600904</v>
       </c>
       <c r="AK89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:AK$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,AK$7))</f>
-        <v>7.4175979302705516E-2</v>
+        <v>0.14835195860541103</v>
       </c>
       <c r="AL89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:AL$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,AL$7))</f>
-        <v>7.4387807163513009E-2</v>
+        <v>0.14877561432702602</v>
       </c>
       <c r="AM89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:AM$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,AM$7))</f>
-        <v>7.4545514888131187E-2</v>
+        <v>0.14909102977626237</v>
       </c>
       <c r="AN89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:AN$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,AN$7))</f>
-        <v>7.4662779512929406E-2</v>
+        <v>0.14932555902585881</v>
       </c>
       <c r="AO89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:AO$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,AO$7))</f>
-        <v>7.4749889451943996E-2</v>
+        <v>0.14949977890388799</v>
       </c>
       <c r="AP89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:AP$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,AP$7))</f>
-        <v>7.4814553263252398E-2</v>
+        <v>0.1496291065265048</v>
       </c>
     </row>
     <row r="90" spans="1:42" x14ac:dyDescent="0.45">
@@ -26586,139 +26579,139 @@
       </c>
       <c r="B3">
         <f>'India Data'!H16</f>
-        <v>0</v>
+        <v>2.6163522012578631E-2</v>
       </c>
       <c r="C3">
         <f>'India Data'!I16</f>
-        <v>0</v>
+        <v>2.5778764335922966E-2</v>
       </c>
       <c r="D3">
         <f>'India Data'!J16</f>
-        <v>0</v>
+        <v>2.5394006659267387E-2</v>
       </c>
       <c r="E3">
         <f>'India Data'!K16</f>
-        <v>0</v>
+        <v>2.5009248982611809E-2</v>
       </c>
       <c r="F3">
         <f>'India Data'!L16</f>
-        <v>0</v>
+        <v>2.4624491305956231E-2</v>
       </c>
       <c r="G3">
         <f>'India Data'!M16</f>
-        <v>0</v>
+        <v>2.4239733629300764E-2</v>
       </c>
       <c r="H3">
         <f>'India Data'!N16</f>
-        <v>0</v>
+        <v>2.3854975952645185E-2</v>
       </c>
       <c r="I3">
         <f>'India Data'!O16</f>
-        <v>0</v>
+        <v>2.3470218275989607E-2</v>
       </c>
       <c r="J3">
         <f>'India Data'!P16</f>
-        <v>0</v>
+        <v>2.3085460599334029E-2</v>
       </c>
       <c r="K3">
         <f>'India Data'!Q16</f>
-        <v>0</v>
+        <v>2.2700702922678451E-2</v>
       </c>
       <c r="L3">
         <f>'India Data'!R16</f>
-        <v>0</v>
+        <v>2.2315945246022872E-2</v>
       </c>
       <c r="M3">
         <f>'India Data'!S16</f>
-        <v>0</v>
+        <v>2.1931187569367294E-2</v>
       </c>
       <c r="N3">
         <f>'India Data'!T16</f>
-        <v>0</v>
+        <v>2.1546429892711716E-2</v>
       </c>
       <c r="O3">
         <f>'India Data'!U16</f>
-        <v>0</v>
+        <v>2.1161672216056138E-2</v>
       </c>
       <c r="P3">
         <f>'India Data'!V16</f>
-        <v>0</v>
+        <v>2.0776914539400559E-2</v>
       </c>
       <c r="Q3">
         <f>'India Data'!W16</f>
-        <v>0</v>
+        <v>2.0392156862744981E-2</v>
       </c>
       <c r="R3">
         <f>'India Data'!X16</f>
-        <v>0</v>
+        <v>2.0007399186089514E-2</v>
       </c>
       <c r="S3">
         <f>'India Data'!Y16</f>
-        <v>0</v>
+        <v>1.9622641509433936E-2</v>
       </c>
       <c r="T3">
         <f>'India Data'!Z16</f>
-        <v>0</v>
+        <v>1.9237883832778357E-2</v>
       </c>
       <c r="U3">
         <f>'India Data'!AA16</f>
-        <v>0</v>
+        <v>1.8853126156122779E-2</v>
       </c>
       <c r="V3">
         <f>'India Data'!AB16</f>
-        <v>0</v>
+        <v>1.8468368479467201E-2</v>
       </c>
       <c r="W3">
         <f>'India Data'!AC16</f>
-        <v>0</v>
+        <v>1.8083610802811623E-2</v>
       </c>
       <c r="X3">
         <f>'India Data'!AD16</f>
-        <v>0</v>
+        <v>1.7698853126156044E-2</v>
       </c>
       <c r="Y3">
         <f>'India Data'!AE16</f>
-        <v>0</v>
+        <v>1.7314095449500466E-2</v>
       </c>
       <c r="Z3">
         <f>'India Data'!AF16</f>
-        <v>0</v>
+        <v>1.6929337772844888E-2</v>
       </c>
       <c r="AA3">
         <f>'India Data'!AG16</f>
-        <v>0</v>
+        <v>1.654458009618931E-2</v>
       </c>
       <c r="AB3">
         <f>'India Data'!AH16</f>
-        <v>0</v>
+        <v>1.6159822419533731E-2</v>
       </c>
       <c r="AC3">
         <f>'India Data'!AI16</f>
-        <v>0</v>
+        <v>1.5775064742878264E-2</v>
       </c>
       <c r="AD3">
         <f>'India Data'!AJ16</f>
-        <v>0</v>
+        <v>1.5390307066222686E-2</v>
       </c>
       <c r="AE3">
         <f>'India Data'!AK16</f>
-        <v>0</v>
+        <v>1.5005549389567108E-2</v>
       </c>
       <c r="AF3">
         <f>'India Data'!AL16</f>
-        <v>0</v>
+        <v>1.4620791712911529E-2</v>
       </c>
       <c r="AG3">
         <f>'India Data'!AM16</f>
-        <v>0</v>
+        <v>1.4236034036255951E-2</v>
       </c>
       <c r="AH3">
         <f>'India Data'!AN16</f>
-        <v>0</v>
+        <v>1.3851276359600373E-2</v>
       </c>
       <c r="AI3">
         <f>'India Data'!AO16</f>
-        <v>0</v>
+        <v>1.3466518682944795E-2</v>
       </c>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.45">
@@ -27013,135 +27006,135 @@
       </c>
       <c r="C6">
         <f>'India Data'!I19</f>
-        <v>1.488022930055813E-3</v>
+        <v>0</v>
       </c>
       <c r="D6">
         <f>'India Data'!J19</f>
-        <v>1.9947745182649396E-3</v>
+        <v>0</v>
       </c>
       <c r="E6">
         <f>'India Data'!K19</f>
-        <v>2.6678391954477131E-3</v>
+        <v>0</v>
       </c>
       <c r="F6">
         <f>'India Data'!L19</f>
-        <v>3.5569404883175086E-3</v>
+        <v>0</v>
       </c>
       <c r="G6">
         <f>'India Data'!M19</f>
-        <v>4.7230017042747376E-3</v>
+        <v>0</v>
       </c>
       <c r="H6">
         <f>'India Data'!N19</f>
-        <v>6.2379522370441774E-3</v>
+        <v>0</v>
       </c>
       <c r="I6">
         <f>'India Data'!O19</f>
-        <v>8.182261589670968E-3</v>
+        <v>0</v>
       </c>
       <c r="J6">
         <f>'India Data'!P19</f>
-        <v>1.0638829867536587E-2</v>
+        <v>0</v>
       </c>
       <c r="K6">
         <f>'India Data'!Q19</f>
-        <v>1.3681914285476725E-2</v>
+        <v>0</v>
       </c>
       <c r="L6">
         <f>'India Data'!R19</f>
-        <v>1.7360641237573676E-2</v>
+        <v>0</v>
       </c>
       <c r="M6">
         <f>'India Data'!S19</f>
-        <v>2.1678787303124704E-2</v>
+        <v>0</v>
       </c>
       <c r="N6">
         <f>'India Data'!T19</f>
-        <v>2.657577703306534E-2</v>
+        <v>0</v>
       </c>
       <c r="O6">
         <f>'India Data'!U19</f>
-        <v>3.1916811239125577E-2</v>
+        <v>0</v>
       </c>
       <c r="P6">
         <f>'India Data'!V19</f>
-        <v>3.7499999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="Q6">
         <f>'India Data'!W19</f>
-        <v>4.3083188760874427E-2</v>
+        <v>0</v>
       </c>
       <c r="R6">
         <f>'India Data'!X19</f>
-        <v>4.8424222966934653E-2</v>
+        <v>0</v>
       </c>
       <c r="S6">
         <f>'India Data'!Y19</f>
-        <v>5.3321212696875293E-2</v>
+        <v>0</v>
       </c>
       <c r="T6">
         <f>'India Data'!Z19</f>
-        <v>5.7639358762426318E-2</v>
+        <v>0</v>
       </c>
       <c r="U6">
         <f>'India Data'!AA19</f>
-        <v>6.1318085714523268E-2</v>
+        <v>0</v>
       </c>
       <c r="V6">
         <f>'India Data'!AB19</f>
-        <v>6.4361170132463424E-2</v>
+        <v>0</v>
       </c>
       <c r="W6">
         <f>'India Data'!AC19</f>
-        <v>6.6817738410329036E-2</v>
+        <v>0</v>
       </c>
       <c r="X6">
         <f>'India Data'!AD19</f>
-        <v>6.8762047762955816E-2</v>
+        <v>0</v>
       </c>
       <c r="Y6">
         <f>'India Data'!AE19</f>
-        <v>7.0276998295725257E-2</v>
+        <v>0</v>
       </c>
       <c r="Z6">
         <f>'India Data'!AF19</f>
-        <v>7.1443059511682491E-2</v>
+        <v>0</v>
       </c>
       <c r="AA6">
         <f>'India Data'!AG19</f>
-        <v>7.2332160804552292E-2</v>
+        <v>0</v>
       </c>
       <c r="AB6">
         <f>'India Data'!AH19</f>
-        <v>7.3005225481735048E-2</v>
+        <v>0</v>
       </c>
       <c r="AC6">
         <f>'India Data'!AI19</f>
-        <v>7.3511977069944182E-2</v>
+        <v>0</v>
       </c>
       <c r="AD6">
         <f>'India Data'!AJ19</f>
-        <v>7.3891947623004522E-2</v>
+        <v>0</v>
       </c>
       <c r="AE6">
         <f>'India Data'!AK19</f>
-        <v>7.4175979302705516E-2</v>
+        <v>0</v>
       </c>
       <c r="AF6">
         <f>'India Data'!AL19</f>
-        <v>7.4387807163513009E-2</v>
+        <v>0</v>
       </c>
       <c r="AG6">
         <f>'India Data'!AM19</f>
-        <v>7.4545514888131187E-2</v>
+        <v>0</v>
       </c>
       <c r="AH6">
         <f>'India Data'!AN19</f>
-        <v>7.4662779512929406E-2</v>
+        <v>0</v>
       </c>
       <c r="AI6">
         <f>'India Data'!AO19</f>
-        <v>7.4749889451943996E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.45">
@@ -28128,135 +28121,135 @@
       </c>
       <c r="C6">
         <f>'India Data'!I26</f>
-        <v>5.9520917202232522E-3</v>
+        <v>0</v>
       </c>
       <c r="D6">
         <f>'India Data'!J26</f>
-        <v>7.9790980730597583E-3</v>
+        <v>0</v>
       </c>
       <c r="E6">
         <f>'India Data'!K26</f>
-        <v>1.0671356781790852E-2</v>
+        <v>0</v>
       </c>
       <c r="F6">
         <f>'India Data'!L26</f>
-        <v>1.4227761953270034E-2</v>
+        <v>0</v>
       </c>
       <c r="G6">
         <f>'India Data'!M26</f>
-        <v>1.889200681709895E-2</v>
+        <v>0</v>
       </c>
       <c r="H6">
         <f>'India Data'!N26</f>
-        <v>2.495180894817671E-2</v>
+        <v>0</v>
       </c>
       <c r="I6">
         <f>'India Data'!O26</f>
-        <v>3.2729046358683872E-2</v>
+        <v>0</v>
       </c>
       <c r="J6">
         <f>'India Data'!P26</f>
-        <v>4.2555319470146347E-2</v>
+        <v>0</v>
       </c>
       <c r="K6">
         <f>'India Data'!Q26</f>
-        <v>5.4727657141906902E-2</v>
+        <v>0</v>
       </c>
       <c r="L6">
         <f>'India Data'!R26</f>
-        <v>6.9442564950294702E-2</v>
+        <v>0</v>
       </c>
       <c r="M6">
         <f>'India Data'!S26</f>
-        <v>8.6715149212498815E-2</v>
+        <v>0</v>
       </c>
       <c r="N6">
         <f>'India Data'!T26</f>
-        <v>0.10630310813226136</v>
+        <v>0</v>
       </c>
       <c r="O6">
         <f>'India Data'!U26</f>
-        <v>0.12766724495650231</v>
+        <v>0</v>
       </c>
       <c r="P6">
         <f>'India Data'!V26</f>
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="Q6">
         <f>'India Data'!W26</f>
-        <v>0.17233275504349771</v>
+        <v>0</v>
       </c>
       <c r="R6">
         <f>'India Data'!X26</f>
-        <v>0.19369689186773861</v>
+        <v>0</v>
       </c>
       <c r="S6">
         <f>'India Data'!Y26</f>
-        <v>0.21328485078750117</v>
+        <v>0</v>
       </c>
       <c r="T6">
         <f>'India Data'!Z26</f>
-        <v>0.23055743504970527</v>
+        <v>0</v>
       </c>
       <c r="U6">
         <f>'India Data'!AA26</f>
-        <v>0.24527234285809307</v>
+        <v>0</v>
       </c>
       <c r="V6">
         <f>'India Data'!AB26</f>
-        <v>0.2574446805298537</v>
+        <v>0</v>
       </c>
       <c r="W6">
         <f>'India Data'!AC26</f>
-        <v>0.26727095364131614</v>
+        <v>0</v>
       </c>
       <c r="X6">
         <f>'India Data'!AD26</f>
-        <v>0.27504819105182327</v>
+        <v>0</v>
       </c>
       <c r="Y6">
         <f>'India Data'!AE26</f>
-        <v>0.28110799318290103</v>
+        <v>0</v>
       </c>
       <c r="Z6">
         <f>'India Data'!AF26</f>
-        <v>0.28577223804672996</v>
+        <v>0</v>
       </c>
       <c r="AA6">
         <f>'India Data'!AG26</f>
-        <v>0.28932864321820917</v>
+        <v>0</v>
       </c>
       <c r="AB6">
         <f>'India Data'!AH26</f>
-        <v>0.29202090192694019</v>
+        <v>0</v>
       </c>
       <c r="AC6">
         <f>'India Data'!AI26</f>
-        <v>0.29404790827977673</v>
+        <v>0</v>
       </c>
       <c r="AD6">
         <f>'India Data'!AJ26</f>
-        <v>0.29556779049201809</v>
+        <v>0</v>
       </c>
       <c r="AE6">
         <f>'India Data'!AK26</f>
-        <v>0.29670391721082207</v>
+        <v>0</v>
       </c>
       <c r="AF6">
         <f>'India Data'!AL26</f>
-        <v>0.29755122865405204</v>
+        <v>0</v>
       </c>
       <c r="AG6">
         <f>'India Data'!AM26</f>
-        <v>0.29818205955252475</v>
+        <v>0</v>
       </c>
       <c r="AH6">
         <f>'India Data'!AN26</f>
-        <v>0.29865111805171762</v>
+        <v>0</v>
       </c>
       <c r="AI6">
         <f>'India Data'!AO26</f>
-        <v>0.29899955780777598</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.45">
@@ -29241,135 +29234,135 @@
       </c>
       <c r="C6">
         <f>'India Data'!I33</f>
-        <v>1.488022930055813E-3</v>
+        <v>0</v>
       </c>
       <c r="D6">
         <f>'India Data'!J33</f>
-        <v>1.9947745182649396E-3</v>
+        <v>0</v>
       </c>
       <c r="E6">
         <f>'India Data'!K33</f>
-        <v>2.6678391954477131E-3</v>
+        <v>0</v>
       </c>
       <c r="F6">
         <f>'India Data'!L33</f>
-        <v>3.5569404883175086E-3</v>
+        <v>0</v>
       </c>
       <c r="G6">
         <f>'India Data'!M33</f>
-        <v>4.7230017042747376E-3</v>
+        <v>0</v>
       </c>
       <c r="H6">
         <f>'India Data'!N33</f>
-        <v>6.2379522370441774E-3</v>
+        <v>0</v>
       </c>
       <c r="I6">
         <f>'India Data'!O33</f>
-        <v>8.182261589670968E-3</v>
+        <v>0</v>
       </c>
       <c r="J6">
         <f>'India Data'!P33</f>
-        <v>1.0638829867536587E-2</v>
+        <v>0</v>
       </c>
       <c r="K6">
         <f>'India Data'!Q33</f>
-        <v>1.3681914285476725E-2</v>
+        <v>0</v>
       </c>
       <c r="L6">
         <f>'India Data'!R33</f>
-        <v>1.7360641237573676E-2</v>
+        <v>0</v>
       </c>
       <c r="M6">
         <f>'India Data'!S33</f>
-        <v>2.1678787303124704E-2</v>
+        <v>0</v>
       </c>
       <c r="N6">
         <f>'India Data'!T33</f>
-        <v>2.657577703306534E-2</v>
+        <v>0</v>
       </c>
       <c r="O6">
         <f>'India Data'!U33</f>
-        <v>3.1916811239125577E-2</v>
+        <v>0</v>
       </c>
       <c r="P6">
         <f>'India Data'!V33</f>
-        <v>3.7499999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="Q6">
         <f>'India Data'!W33</f>
-        <v>4.3083188760874427E-2</v>
+        <v>0</v>
       </c>
       <c r="R6">
         <f>'India Data'!X33</f>
-        <v>4.8424222966934653E-2</v>
+        <v>0</v>
       </c>
       <c r="S6">
         <f>'India Data'!Y33</f>
-        <v>5.3321212696875293E-2</v>
+        <v>0</v>
       </c>
       <c r="T6">
         <f>'India Data'!Z33</f>
-        <v>5.7639358762426318E-2</v>
+        <v>0</v>
       </c>
       <c r="U6">
         <f>'India Data'!AA33</f>
-        <v>6.1318085714523268E-2</v>
+        <v>0</v>
       </c>
       <c r="V6">
         <f>'India Data'!AB33</f>
-        <v>6.4361170132463424E-2</v>
+        <v>0</v>
       </c>
       <c r="W6">
         <f>'India Data'!AC33</f>
-        <v>6.6817738410329036E-2</v>
+        <v>0</v>
       </c>
       <c r="X6">
         <f>'India Data'!AD33</f>
-        <v>6.8762047762955816E-2</v>
+        <v>0</v>
       </c>
       <c r="Y6">
         <f>'India Data'!AE33</f>
-        <v>7.0276998295725257E-2</v>
+        <v>0</v>
       </c>
       <c r="Z6">
         <f>'India Data'!AF33</f>
-        <v>7.1443059511682491E-2</v>
+        <v>0</v>
       </c>
       <c r="AA6">
         <f>'India Data'!AG33</f>
-        <v>7.2332160804552292E-2</v>
+        <v>0</v>
       </c>
       <c r="AB6">
         <f>'India Data'!AH33</f>
-        <v>7.3005225481735048E-2</v>
+        <v>0</v>
       </c>
       <c r="AC6">
         <f>'India Data'!AI33</f>
-        <v>7.3511977069944182E-2</v>
+        <v>0</v>
       </c>
       <c r="AD6">
         <f>'India Data'!AJ33</f>
-        <v>7.3891947623004522E-2</v>
+        <v>0</v>
       </c>
       <c r="AE6">
         <f>'India Data'!AK33</f>
-        <v>7.4175979302705516E-2</v>
+        <v>0</v>
       </c>
       <c r="AF6">
         <f>'India Data'!AL33</f>
-        <v>7.4387807163513009E-2</v>
+        <v>0</v>
       </c>
       <c r="AG6">
         <f>'India Data'!AM33</f>
-        <v>7.4545514888131187E-2</v>
+        <v>0</v>
       </c>
       <c r="AH6">
         <f>'India Data'!AN33</f>
-        <v>7.4662779512929406E-2</v>
+        <v>0</v>
       </c>
       <c r="AI6">
         <f>'India Data'!AO33</f>
-        <v>7.4749889451943996E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Additional MPNVbT calibration edits
</commit_message>
<xml_diff>
--- a/InputData/trans/MPNVbT/Max Perc New Veh by Technology.xlsx
+++ b/InputData/trans/MPNVbT/Max Perc New Veh by Technology.xlsx
@@ -678,6 +678,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10703,135 +10704,135 @@
       </c>
       <c r="C6">
         <f>'India Data'!I89</f>
-        <v>2.9760458601116261E-3</v>
+        <v>0</v>
       </c>
       <c r="D6">
         <f>'India Data'!J89</f>
-        <v>3.9895490365298792E-3</v>
+        <v>0</v>
       </c>
       <c r="E6">
         <f>'India Data'!K89</f>
-        <v>5.3356783908954262E-3</v>
+        <v>0</v>
       </c>
       <c r="F6">
         <f>'India Data'!L89</f>
-        <v>7.1138809766350172E-3</v>
+        <v>0</v>
       </c>
       <c r="G6">
         <f>'India Data'!M89</f>
-        <v>9.4460034085494752E-3</v>
+        <v>0</v>
       </c>
       <c r="H6">
         <f>'India Data'!N89</f>
-        <v>1.2475904474088355E-2</v>
+        <v>0</v>
       </c>
       <c r="I6">
         <f>'India Data'!O89</f>
-        <v>1.6364523179341936E-2</v>
+        <v>0</v>
       </c>
       <c r="J6">
         <f>'India Data'!P89</f>
-        <v>2.1277659735073173E-2</v>
+        <v>0</v>
       </c>
       <c r="K6">
         <f>'India Data'!Q89</f>
-        <v>2.7363828570953451E-2</v>
+        <v>0</v>
       </c>
       <c r="L6">
         <f>'India Data'!R89</f>
-        <v>3.4721282475147351E-2</v>
+        <v>0</v>
       </c>
       <c r="M6">
         <f>'India Data'!S89</f>
-        <v>4.3357574606249408E-2</v>
+        <v>0</v>
       </c>
       <c r="N6">
         <f>'India Data'!T89</f>
-        <v>5.3151554066130681E-2</v>
+        <v>0</v>
       </c>
       <c r="O6">
         <f>'India Data'!U89</f>
-        <v>6.3833622478251154E-2</v>
+        <v>0</v>
       </c>
       <c r="P6">
         <f>'India Data'!V89</f>
-        <v>7.4999999999999997E-2</v>
+        <v>0</v>
       </c>
       <c r="Q6">
         <f>'India Data'!W89</f>
-        <v>8.6166377521748855E-2</v>
+        <v>0</v>
       </c>
       <c r="R6">
         <f>'India Data'!X89</f>
-        <v>9.6848445933869307E-2</v>
+        <v>0</v>
       </c>
       <c r="S6">
         <f>'India Data'!Y89</f>
-        <v>0.10664242539375059</v>
+        <v>0</v>
       </c>
       <c r="T6">
         <f>'India Data'!Z89</f>
-        <v>0.11527871752485264</v>
+        <v>0</v>
       </c>
       <c r="U6">
         <f>'India Data'!AA89</f>
-        <v>0.12263617142904654</v>
+        <v>0</v>
       </c>
       <c r="V6">
         <f>'India Data'!AB89</f>
-        <v>0.12872234026492685</v>
+        <v>0</v>
       </c>
       <c r="W6">
         <f>'India Data'!AC89</f>
-        <v>0.13363547682065807</v>
+        <v>0</v>
       </c>
       <c r="X6">
         <f>'India Data'!AD89</f>
-        <v>0.13752409552591163</v>
+        <v>0</v>
       </c>
       <c r="Y6">
         <f>'India Data'!AE89</f>
-        <v>0.14055399659145051</v>
+        <v>0</v>
       </c>
       <c r="Z6">
         <f>'India Data'!AF89</f>
-        <v>0.14288611902336498</v>
+        <v>0</v>
       </c>
       <c r="AA6">
         <f>'India Data'!AG89</f>
-        <v>0.14466432160910458</v>
+        <v>0</v>
       </c>
       <c r="AB6">
         <f>'India Data'!AH89</f>
-        <v>0.1460104509634701</v>
+        <v>0</v>
       </c>
       <c r="AC6">
         <f>'India Data'!AI89</f>
-        <v>0.14702395413988836</v>
+        <v>0</v>
       </c>
       <c r="AD6">
         <f>'India Data'!AJ89</f>
-        <v>0.14778389524600904</v>
+        <v>0</v>
       </c>
       <c r="AE6">
         <f>'India Data'!AK89</f>
-        <v>0.14835195860541103</v>
+        <v>0</v>
       </c>
       <c r="AF6">
         <f>'India Data'!AL89</f>
-        <v>0.14877561432702602</v>
+        <v>0</v>
       </c>
       <c r="AG6">
         <f>'India Data'!AM89</f>
-        <v>0.14909102977626237</v>
+        <v>0</v>
       </c>
       <c r="AH6">
         <f>'India Data'!AN89</f>
-        <v>0.14932555902585881</v>
+        <v>0</v>
       </c>
       <c r="AI6">
         <f>'India Data'!AO89</f>
-        <v>0.14949977890388799</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.45">
@@ -11744,8 +11745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="E90" sqref="E90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -15290,7 +15291,7 @@
         <v>0</v>
       </c>
       <c r="E29" s="10">
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
       <c r="F29" s="15" t="str">
         <f t="shared" si="4"/>
@@ -15302,139 +15303,139 @@
       </c>
       <c r="I29">
         <f>IF($F29="s-curve",$D29+($E29-$D29)*$I$2/(1+EXP($I$3*(COUNT($H$7:I$7)+$I$4))),TREND($D29:$E29,$D$7:$E$7,I$7))</f>
-        <v>2.9760458601116261E-3</v>
+        <v>7.9361222936310042E-4</v>
       </c>
       <c r="J29">
         <f>IF($F29="s-curve",$D29+($E29-$D29)*$I$2/(1+EXP($I$3*(COUNT($H$7:J$7)+$I$4))),TREND($D29:$E29,$D$7:$E$7,J$7))</f>
-        <v>3.9895490365298792E-3</v>
+        <v>1.0638797430746346E-3</v>
       </c>
       <c r="K29">
         <f>IF($F29="s-curve",$D29+($E29-$D29)*$I$2/(1+EXP($I$3*(COUNT($H$7:K$7)+$I$4))),TREND($D29:$E29,$D$7:$E$7,K$7))</f>
-        <v>5.3356783908954262E-3</v>
+        <v>1.4228475709054471E-3</v>
       </c>
       <c r="L29">
         <f>IF($F29="s-curve",$D29+($E29-$D29)*$I$2/(1+EXP($I$3*(COUNT($H$7:L$7)+$I$4))),TREND($D29:$E29,$D$7:$E$7,L$7))</f>
-        <v>7.1138809766350172E-3</v>
+        <v>1.8970349271026712E-3</v>
       </c>
       <c r="M29">
         <f>IF($F29="s-curve",$D29+($E29-$D29)*$I$2/(1+EXP($I$3*(COUNT($H$7:M$7)+$I$4))),TREND($D29:$E29,$D$7:$E$7,M$7))</f>
-        <v>9.4460034085494752E-3</v>
+        <v>2.5189342422798603E-3</v>
       </c>
       <c r="N29">
         <f>IF($F29="s-curve",$D29+($E29-$D29)*$I$2/(1+EXP($I$3*(COUNT($H$7:N$7)+$I$4))),TREND($D29:$E29,$D$7:$E$7,N$7))</f>
-        <v>1.2475904474088355E-2</v>
+        <v>3.3269078597568951E-3</v>
       </c>
       <c r="O29">
         <f>IF($F29="s-curve",$D29+($E29-$D29)*$I$2/(1+EXP($I$3*(COUNT($H$7:O$7)+$I$4))),TREND($D29:$E29,$D$7:$E$7,O$7))</f>
-        <v>1.6364523179341936E-2</v>
+        <v>4.3638728478245167E-3</v>
       </c>
       <c r="P29">
         <f>IF($F29="s-curve",$D29+($E29-$D29)*$I$2/(1+EXP($I$3*(COUNT($H$7:P$7)+$I$4))),TREND($D29:$E29,$D$7:$E$7,P$7))</f>
-        <v>2.1277659735073173E-2</v>
+        <v>5.6740425960195131E-3</v>
       </c>
       <c r="Q29">
         <f>IF($F29="s-curve",$D29+($E29-$D29)*$I$2/(1+EXP($I$3*(COUNT($H$7:Q$7)+$I$4))),TREND($D29:$E29,$D$7:$E$7,Q$7))</f>
-        <v>2.7363828570953451E-2</v>
+        <v>7.2970209522542542E-3</v>
       </c>
       <c r="R29">
         <f>IF($F29="s-curve",$D29+($E29-$D29)*$I$2/(1+EXP($I$3*(COUNT($H$7:R$7)+$I$4))),TREND($D29:$E29,$D$7:$E$7,R$7))</f>
-        <v>3.4721282475147351E-2</v>
+        <v>9.2590086600392949E-3</v>
       </c>
       <c r="S29">
         <f>IF($F29="s-curve",$D29+($E29-$D29)*$I$2/(1+EXP($I$3*(COUNT($H$7:S$7)+$I$4))),TREND($D29:$E29,$D$7:$E$7,S$7))</f>
-        <v>4.3357574606249408E-2</v>
+        <v>1.1562019894999843E-2</v>
       </c>
       <c r="T29">
         <f>IF($F29="s-curve",$D29+($E29-$D29)*$I$2/(1+EXP($I$3*(COUNT($H$7:T$7)+$I$4))),TREND($D29:$E29,$D$7:$E$7,T$7))</f>
-        <v>5.3151554066130681E-2</v>
+        <v>1.4173747750968182E-2</v>
       </c>
       <c r="U29">
         <f>IF($F29="s-curve",$D29+($E29-$D29)*$I$2/(1+EXP($I$3*(COUNT($H$7:U$7)+$I$4))),TREND($D29:$E29,$D$7:$E$7,U$7))</f>
-        <v>6.3833622478251154E-2</v>
+        <v>1.702229932753364E-2</v>
       </c>
       <c r="V29">
         <f>IF($F29="s-curve",$D29+($E29-$D29)*$I$2/(1+EXP($I$3*(COUNT($H$7:V$7)+$I$4))),TREND($D29:$E29,$D$7:$E$7,V$7))</f>
-        <v>7.4999999999999997E-2</v>
+        <v>0.02</v>
       </c>
       <c r="W29">
         <f>IF($F29="s-curve",$D29+($E29-$D29)*$I$2/(1+EXP($I$3*(COUNT($H$7:W$7)+$I$4))),TREND($D29:$E29,$D$7:$E$7,W$7))</f>
-        <v>8.6166377521748855E-2</v>
+        <v>2.2977700672466361E-2</v>
       </c>
       <c r="X29">
         <f>IF($F29="s-curve",$D29+($E29-$D29)*$I$2/(1+EXP($I$3*(COUNT($H$7:X$7)+$I$4))),TREND($D29:$E29,$D$7:$E$7,X$7))</f>
-        <v>9.6848445933869307E-2</v>
+        <v>2.5826252249031817E-2</v>
       </c>
       <c r="Y29">
         <f>IF($F29="s-curve",$D29+($E29-$D29)*$I$2/(1+EXP($I$3*(COUNT($H$7:Y$7)+$I$4))),TREND($D29:$E29,$D$7:$E$7,Y$7))</f>
-        <v>0.10664242539375059</v>
+        <v>2.8437980105000156E-2</v>
       </c>
       <c r="Z29">
         <f>IF($F29="s-curve",$D29+($E29-$D29)*$I$2/(1+EXP($I$3*(COUNT($H$7:Z$7)+$I$4))),TREND($D29:$E29,$D$7:$E$7,Z$7))</f>
-        <v>0.11527871752485264</v>
+        <v>3.0740991339960704E-2</v>
       </c>
       <c r="AA29">
         <f>IF($F29="s-curve",$D29+($E29-$D29)*$I$2/(1+EXP($I$3*(COUNT($H$7:AA$7)+$I$4))),TREND($D29:$E29,$D$7:$E$7,AA$7))</f>
-        <v>0.12263617142904654</v>
+        <v>3.2702979047745745E-2</v>
       </c>
       <c r="AB29">
         <f>IF($F29="s-curve",$D29+($E29-$D29)*$I$2/(1+EXP($I$3*(COUNT($H$7:AB$7)+$I$4))),TREND($D29:$E29,$D$7:$E$7,AB$7))</f>
-        <v>0.12872234026492685</v>
+        <v>3.4325957403980492E-2</v>
       </c>
       <c r="AC29">
         <f>IF($F29="s-curve",$D29+($E29-$D29)*$I$2/(1+EXP($I$3*(COUNT($H$7:AC$7)+$I$4))),TREND($D29:$E29,$D$7:$E$7,AC$7))</f>
-        <v>0.13363547682065807</v>
+        <v>3.5636127152175484E-2</v>
       </c>
       <c r="AD29">
         <f>IF($F29="s-curve",$D29+($E29-$D29)*$I$2/(1+EXP($I$3*(COUNT($H$7:AD$7)+$I$4))),TREND($D29:$E29,$D$7:$E$7,AD$7))</f>
-        <v>0.13752409552591163</v>
+        <v>3.6673092140243106E-2</v>
       </c>
       <c r="AE29">
         <f>IF($F29="s-curve",$D29+($E29-$D29)*$I$2/(1+EXP($I$3*(COUNT($H$7:AE$7)+$I$4))),TREND($D29:$E29,$D$7:$E$7,AE$7))</f>
-        <v>0.14055399659145051</v>
+        <v>3.7481065757720144E-2</v>
       </c>
       <c r="AF29">
         <f>IF($F29="s-curve",$D29+($E29-$D29)*$I$2/(1+EXP($I$3*(COUNT($H$7:AF$7)+$I$4))),TREND($D29:$E29,$D$7:$E$7,AF$7))</f>
-        <v>0.14288611902336498</v>
+        <v>3.8102965072897337E-2</v>
       </c>
       <c r="AG29">
         <f>IF($F29="s-curve",$D29+($E29-$D29)*$I$2/(1+EXP($I$3*(COUNT($H$7:AG$7)+$I$4))),TREND($D29:$E29,$D$7:$E$7,AG$7))</f>
-        <v>0.14466432160910458</v>
+        <v>3.8577152429094555E-2</v>
       </c>
       <c r="AH29">
         <f>IF($F29="s-curve",$D29+($E29-$D29)*$I$2/(1+EXP($I$3*(COUNT($H$7:AH$7)+$I$4))),TREND($D29:$E29,$D$7:$E$7,AH$7))</f>
-        <v>0.1460104509634701</v>
+        <v>3.8936120256925361E-2</v>
       </c>
       <c r="AI29">
         <f>IF($F29="s-curve",$D29+($E29-$D29)*$I$2/(1+EXP($I$3*(COUNT($H$7:AI$7)+$I$4))),TREND($D29:$E29,$D$7:$E$7,AI$7))</f>
-        <v>0.14702395413988836</v>
+        <v>3.9206387770636904E-2</v>
       </c>
       <c r="AJ29">
         <f>IF($F29="s-curve",$D29+($E29-$D29)*$I$2/(1+EXP($I$3*(COUNT($H$7:AJ$7)+$I$4))),TREND($D29:$E29,$D$7:$E$7,AJ$7))</f>
-        <v>0.14778389524600904</v>
+        <v>3.9409038732269079E-2</v>
       </c>
       <c r="AK29">
         <f>IF($F29="s-curve",$D29+($E29-$D29)*$I$2/(1+EXP($I$3*(COUNT($H$7:AK$7)+$I$4))),TREND($D29:$E29,$D$7:$E$7,AK$7))</f>
-        <v>0.14835195860541103</v>
+        <v>3.9560522294776274E-2</v>
       </c>
       <c r="AL29">
         <f>IF($F29="s-curve",$D29+($E29-$D29)*$I$2/(1+EXP($I$3*(COUNT($H$7:AL$7)+$I$4))),TREND($D29:$E29,$D$7:$E$7,AL$7))</f>
-        <v>0.14877561432702602</v>
+        <v>3.9673497153873603E-2</v>
       </c>
       <c r="AM29">
         <f>IF($F29="s-curve",$D29+($E29-$D29)*$I$2/(1+EXP($I$3*(COUNT($H$7:AM$7)+$I$4))),TREND($D29:$E29,$D$7:$E$7,AM$7))</f>
-        <v>0.14909102977626237</v>
+        <v>3.9757607940336635E-2</v>
       </c>
       <c r="AN29">
         <f>IF($F29="s-curve",$D29+($E29-$D29)*$I$2/(1+EXP($I$3*(COUNT($H$7:AN$7)+$I$4))),TREND($D29:$E29,$D$7:$E$7,AN$7))</f>
-        <v>0.14932555902585881</v>
+        <v>3.9820149073562357E-2</v>
       </c>
       <c r="AO29">
         <f>IF($F29="s-curve",$D29+($E29-$D29)*$I$2/(1+EXP($I$3*(COUNT($H$7:AO$7)+$I$4))),TREND($D29:$E29,$D$7:$E$7,AO$7))</f>
-        <v>0.14949977890388799</v>
+        <v>3.9866607707703471E-2</v>
       </c>
       <c r="AP29">
         <f>IF($F29="s-curve",$D29+($E29-$D29)*$I$2/(1+EXP($I$3*(COUNT($H$7:AP$7)+$I$4))),TREND($D29:$E29,$D$7:$E$7,AP$7))</f>
-        <v>0.1496291065265048</v>
+        <v>3.9901095073734613E-2</v>
       </c>
     </row>
     <row r="30" spans="1:42" x14ac:dyDescent="0.45">
@@ -24720,12 +24721,11 @@
         <v>0</v>
       </c>
       <c r="E89" s="10">
-        <f>E85*'India Assumptions'!$A$36</f>
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="F89" s="15" t="str">
         <f t="shared" si="10"/>
-        <v>s-curve</v>
+        <v>n/a</v>
       </c>
       <c r="H89" s="10">
         <f t="shared" si="7"/>
@@ -24733,139 +24733,139 @@
       </c>
       <c r="I89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:I$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,I$7))</f>
-        <v>2.9760458601116261E-3</v>
+        <v>0</v>
       </c>
       <c r="J89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:J$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,J$7))</f>
-        <v>3.9895490365298792E-3</v>
+        <v>0</v>
       </c>
       <c r="K89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:K$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,K$7))</f>
-        <v>5.3356783908954262E-3</v>
+        <v>0</v>
       </c>
       <c r="L89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:L$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,L$7))</f>
-        <v>7.1138809766350172E-3</v>
+        <v>0</v>
       </c>
       <c r="M89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:M$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,M$7))</f>
-        <v>9.4460034085494752E-3</v>
+        <v>0</v>
       </c>
       <c r="N89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:N$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,N$7))</f>
-        <v>1.2475904474088355E-2</v>
+        <v>0</v>
       </c>
       <c r="O89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:O$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,O$7))</f>
-        <v>1.6364523179341936E-2</v>
+        <v>0</v>
       </c>
       <c r="P89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:P$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,P$7))</f>
-        <v>2.1277659735073173E-2</v>
+        <v>0</v>
       </c>
       <c r="Q89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:Q$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,Q$7))</f>
-        <v>2.7363828570953451E-2</v>
+        <v>0</v>
       </c>
       <c r="R89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:R$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,R$7))</f>
-        <v>3.4721282475147351E-2</v>
+        <v>0</v>
       </c>
       <c r="S89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:S$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,S$7))</f>
-        <v>4.3357574606249408E-2</v>
+        <v>0</v>
       </c>
       <c r="T89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:T$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,T$7))</f>
-        <v>5.3151554066130681E-2</v>
+        <v>0</v>
       </c>
       <c r="U89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:U$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,U$7))</f>
-        <v>6.3833622478251154E-2</v>
+        <v>0</v>
       </c>
       <c r="V89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:V$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,V$7))</f>
-        <v>7.4999999999999997E-2</v>
+        <v>0</v>
       </c>
       <c r="W89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:W$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,W$7))</f>
-        <v>8.6166377521748855E-2</v>
+        <v>0</v>
       </c>
       <c r="X89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:X$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,X$7))</f>
-        <v>9.6848445933869307E-2</v>
+        <v>0</v>
       </c>
       <c r="Y89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:Y$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,Y$7))</f>
-        <v>0.10664242539375059</v>
+        <v>0</v>
       </c>
       <c r="Z89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:Z$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,Z$7))</f>
-        <v>0.11527871752485264</v>
+        <v>0</v>
       </c>
       <c r="AA89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:AA$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,AA$7))</f>
-        <v>0.12263617142904654</v>
+        <v>0</v>
       </c>
       <c r="AB89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:AB$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,AB$7))</f>
-        <v>0.12872234026492685</v>
+        <v>0</v>
       </c>
       <c r="AC89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:AC$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,AC$7))</f>
-        <v>0.13363547682065807</v>
+        <v>0</v>
       </c>
       <c r="AD89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:AD$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,AD$7))</f>
-        <v>0.13752409552591163</v>
+        <v>0</v>
       </c>
       <c r="AE89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:AE$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,AE$7))</f>
-        <v>0.14055399659145051</v>
+        <v>0</v>
       </c>
       <c r="AF89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:AF$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,AF$7))</f>
-        <v>0.14288611902336498</v>
+        <v>0</v>
       </c>
       <c r="AG89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:AG$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,AG$7))</f>
-        <v>0.14466432160910458</v>
+        <v>0</v>
       </c>
       <c r="AH89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:AH$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,AH$7))</f>
-        <v>0.1460104509634701</v>
+        <v>0</v>
       </c>
       <c r="AI89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:AI$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,AI$7))</f>
-        <v>0.14702395413988836</v>
+        <v>0</v>
       </c>
       <c r="AJ89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:AJ$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,AJ$7))</f>
-        <v>0.14778389524600904</v>
+        <v>0</v>
       </c>
       <c r="AK89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:AK$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,AK$7))</f>
-        <v>0.14835195860541103</v>
+        <v>0</v>
       </c>
       <c r="AL89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:AL$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,AL$7))</f>
-        <v>0.14877561432702602</v>
+        <v>0</v>
       </c>
       <c r="AM89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:AM$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,AM$7))</f>
-        <v>0.14909102977626237</v>
+        <v>0</v>
       </c>
       <c r="AN89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:AN$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,AN$7))</f>
-        <v>0.14932555902585881</v>
+        <v>0</v>
       </c>
       <c r="AO89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:AO$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,AO$7))</f>
-        <v>0.14949977890388799</v>
+        <v>0</v>
       </c>
       <c r="AP89">
         <f>IF($F89="s-curve",$D89+($E89-$D89)*$I$2/(1+EXP($I$3*(COUNT($H$7:AP$7)+$I$4))),TREND($D89:$E89,$D$7:$E$7,AP$7))</f>
-        <v>0.1496291065265048</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:42" x14ac:dyDescent="0.45">
@@ -28670,135 +28670,135 @@
       </c>
       <c r="C2">
         <f>'India Data'!I29</f>
-        <v>2.9760458601116261E-3</v>
+        <v>7.9361222936310042E-4</v>
       </c>
       <c r="D2">
         <f>'India Data'!J29</f>
-        <v>3.9895490365298792E-3</v>
+        <v>1.0638797430746346E-3</v>
       </c>
       <c r="E2">
         <f>'India Data'!K29</f>
-        <v>5.3356783908954262E-3</v>
+        <v>1.4228475709054471E-3</v>
       </c>
       <c r="F2">
         <f>'India Data'!L29</f>
-        <v>7.1138809766350172E-3</v>
+        <v>1.8970349271026712E-3</v>
       </c>
       <c r="G2">
         <f>'India Data'!M29</f>
-        <v>9.4460034085494752E-3</v>
+        <v>2.5189342422798603E-3</v>
       </c>
       <c r="H2">
         <f>'India Data'!N29</f>
-        <v>1.2475904474088355E-2</v>
+        <v>3.3269078597568951E-3</v>
       </c>
       <c r="I2">
         <f>'India Data'!O29</f>
-        <v>1.6364523179341936E-2</v>
+        <v>4.3638728478245167E-3</v>
       </c>
       <c r="J2">
         <f>'India Data'!P29</f>
-        <v>2.1277659735073173E-2</v>
+        <v>5.6740425960195131E-3</v>
       </c>
       <c r="K2">
         <f>'India Data'!Q29</f>
-        <v>2.7363828570953451E-2</v>
+        <v>7.2970209522542542E-3</v>
       </c>
       <c r="L2">
         <f>'India Data'!R29</f>
-        <v>3.4721282475147351E-2</v>
+        <v>9.2590086600392949E-3</v>
       </c>
       <c r="M2">
         <f>'India Data'!S29</f>
-        <v>4.3357574606249408E-2</v>
+        <v>1.1562019894999843E-2</v>
       </c>
       <c r="N2">
         <f>'India Data'!T29</f>
-        <v>5.3151554066130681E-2</v>
+        <v>1.4173747750968182E-2</v>
       </c>
       <c r="O2">
         <f>'India Data'!U29</f>
-        <v>6.3833622478251154E-2</v>
+        <v>1.702229932753364E-2</v>
       </c>
       <c r="P2">
         <f>'India Data'!V29</f>
-        <v>7.4999999999999997E-2</v>
+        <v>0.02</v>
       </c>
       <c r="Q2">
         <f>'India Data'!W29</f>
-        <v>8.6166377521748855E-2</v>
+        <v>2.2977700672466361E-2</v>
       </c>
       <c r="R2">
         <f>'India Data'!X29</f>
-        <v>9.6848445933869307E-2</v>
+        <v>2.5826252249031817E-2</v>
       </c>
       <c r="S2">
         <f>'India Data'!Y29</f>
-        <v>0.10664242539375059</v>
+        <v>2.8437980105000156E-2</v>
       </c>
       <c r="T2">
         <f>'India Data'!Z29</f>
-        <v>0.11527871752485264</v>
+        <v>3.0740991339960704E-2</v>
       </c>
       <c r="U2">
         <f>'India Data'!AA29</f>
-        <v>0.12263617142904654</v>
+        <v>3.2702979047745745E-2</v>
       </c>
       <c r="V2">
         <f>'India Data'!AB29</f>
-        <v>0.12872234026492685</v>
+        <v>3.4325957403980492E-2</v>
       </c>
       <c r="W2">
         <f>'India Data'!AC29</f>
-        <v>0.13363547682065807</v>
+        <v>3.5636127152175484E-2</v>
       </c>
       <c r="X2">
         <f>'India Data'!AD29</f>
-        <v>0.13752409552591163</v>
+        <v>3.6673092140243106E-2</v>
       </c>
       <c r="Y2">
         <f>'India Data'!AE29</f>
-        <v>0.14055399659145051</v>
+        <v>3.7481065757720144E-2</v>
       </c>
       <c r="Z2">
         <f>'India Data'!AF29</f>
-        <v>0.14288611902336498</v>
+        <v>3.8102965072897337E-2</v>
       </c>
       <c r="AA2">
         <f>'India Data'!AG29</f>
-        <v>0.14466432160910458</v>
+        <v>3.8577152429094555E-2</v>
       </c>
       <c r="AB2">
         <f>'India Data'!AH29</f>
-        <v>0.1460104509634701</v>
+        <v>3.8936120256925361E-2</v>
       </c>
       <c r="AC2">
         <f>'India Data'!AI29</f>
-        <v>0.14702395413988836</v>
+        <v>3.9206387770636904E-2</v>
       </c>
       <c r="AD2">
         <f>'India Data'!AJ29</f>
-        <v>0.14778389524600904</v>
+        <v>3.9409038732269079E-2</v>
       </c>
       <c r="AE2">
         <f>'India Data'!AK29</f>
-        <v>0.14835195860541103</v>
+        <v>3.9560522294776274E-2</v>
       </c>
       <c r="AF2">
         <f>'India Data'!AL29</f>
-        <v>0.14877561432702602</v>
+        <v>3.9673497153873603E-2</v>
       </c>
       <c r="AG2">
         <f>'India Data'!AM29</f>
-        <v>0.14909102977626237</v>
+        <v>3.9757607940336635E-2</v>
       </c>
       <c r="AH2">
         <f>'India Data'!AN29</f>
-        <v>0.14932555902585881</v>
+        <v>3.9820149073562357E-2</v>
       </c>
       <c r="AI2">
         <f>'India Data'!AO29</f>
-        <v>0.14949977890388799</v>
+        <v>3.9866607707703471E-2</v>
       </c>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Update MPNVbT for rail
</commit_message>
<xml_diff>
--- a/InputData/trans/MPNVbT/Max Perc New Veh by Technology.xlsx
+++ b/InputData/trans/MPNVbT/Max Perc New Veh by Technology.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -678,7 +678,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2011,7 +2010,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
@@ -4960,135 +4959,135 @@
       </c>
       <c r="C5">
         <f>'India Data'!I53</f>
-        <v>0.50338235294117339</v>
+        <v>0.49226470588235305</v>
       </c>
       <c r="D5">
         <f>'India Data'!J53</f>
-        <v>0.51776470588234957</v>
+        <v>0.49552941176470622</v>
       </c>
       <c r="E5">
         <f>'India Data'!K53</f>
-        <v>0.53214705882352931</v>
+        <v>0.4987941176470585</v>
       </c>
       <c r="F5">
         <f>'India Data'!L53</f>
-        <v>0.54652941176470549</v>
+        <v>0.50205882352941167</v>
       </c>
       <c r="G5">
         <f>'India Data'!M53</f>
-        <v>0.56091176470588167</v>
+        <v>0.50532352941176484</v>
       </c>
       <c r="H5">
         <f>'India Data'!N53</f>
-        <v>0.57529411764705785</v>
+        <v>0.50858823529411801</v>
       </c>
       <c r="I5">
         <f>'India Data'!O53</f>
-        <v>0.58967647058823403</v>
+        <v>0.51185294117647029</v>
       </c>
       <c r="J5">
         <f>'India Data'!P53</f>
-        <v>0.6040588235294102</v>
+        <v>0.51511764705882346</v>
       </c>
       <c r="K5">
         <f>'India Data'!Q53</f>
-        <v>0.61844117647058638</v>
+        <v>0.51838235294117663</v>
       </c>
       <c r="L5">
         <f>'India Data'!R53</f>
-        <v>0.63282352941176256</v>
+        <v>0.5216470588235298</v>
       </c>
       <c r="M5">
         <f>'India Data'!S53</f>
-        <v>0.64720588235293874</v>
+        <v>0.52491176470588208</v>
       </c>
       <c r="N5">
         <f>'India Data'!T53</f>
-        <v>0.66158823529411492</v>
+        <v>0.52817647058823525</v>
       </c>
       <c r="O5">
         <f>'India Data'!U53</f>
-        <v>0.6759705882352911</v>
+        <v>0.53144117647058842</v>
       </c>
       <c r="P5">
         <f>'India Data'!V53</f>
-        <v>0.69035294117646728</v>
+        <v>0.53470588235294159</v>
       </c>
       <c r="Q5">
         <f>'India Data'!W53</f>
-        <v>0.70473529411764702</v>
+        <v>0.53797058823529387</v>
       </c>
       <c r="R5">
         <f>'India Data'!X53</f>
-        <v>0.7191176470588232</v>
+        <v>0.54123529411764704</v>
       </c>
       <c r="S5">
         <f>'India Data'!Y53</f>
-        <v>0.73349999999999937</v>
+        <v>0.54450000000000021</v>
       </c>
       <c r="T5">
         <f>'India Data'!Z53</f>
-        <v>0.74788235294117555</v>
+        <v>0.54776470588235338</v>
       </c>
       <c r="U5">
         <f>'India Data'!AA53</f>
-        <v>0.76226470588235173</v>
+        <v>0.55102941176470566</v>
       </c>
       <c r="V5">
         <f>'India Data'!AB53</f>
-        <v>0.77664705882352791</v>
+        <v>0.55429411764705883</v>
       </c>
       <c r="W5">
         <f>'India Data'!AC53</f>
-        <v>0.79102941176470409</v>
+        <v>0.557558823529412</v>
       </c>
       <c r="X5">
         <f>'India Data'!AD53</f>
-        <v>0.80541176470588027</v>
+        <v>0.56082352941176516</v>
       </c>
       <c r="Y5">
         <f>'India Data'!AE53</f>
-        <v>0.81979411764705645</v>
+        <v>0.56408823529411745</v>
       </c>
       <c r="Z5">
         <f>'India Data'!AF53</f>
-        <v>0.83417647058823263</v>
+        <v>0.56735294117647062</v>
       </c>
       <c r="AA5">
         <f>'India Data'!AG53</f>
-        <v>0.84855882352940881</v>
+        <v>0.57061764705882378</v>
       </c>
       <c r="AB5">
         <f>'India Data'!AH53</f>
-        <v>0.86294117647058499</v>
+        <v>0.57388235294117695</v>
       </c>
       <c r="AC5">
         <f>'India Data'!AI53</f>
-        <v>0.87732352941176472</v>
+        <v>0.57714705882352924</v>
       </c>
       <c r="AD5">
         <f>'India Data'!AJ53</f>
-        <v>0.8917058823529409</v>
+        <v>0.5804117647058824</v>
       </c>
       <c r="AE5">
         <f>'India Data'!AK53</f>
-        <v>0.90608823529411708</v>
+        <v>0.58367647058823557</v>
       </c>
       <c r="AF5">
         <f>'India Data'!AL53</f>
-        <v>0.92047058823529326</v>
+        <v>0.58694117647058874</v>
       </c>
       <c r="AG5">
         <f>'India Data'!AM53</f>
-        <v>0.93485294117646944</v>
+        <v>0.59020588235294102</v>
       </c>
       <c r="AH5">
         <f>'India Data'!AN53</f>
-        <v>0.94923529411764562</v>
+        <v>0.59347058823529419</v>
       </c>
       <c r="AI5">
         <f>'India Data'!AO53</f>
-        <v>0.9636176470588218</v>
+        <v>0.59673529411764736</v>
       </c>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.45">
@@ -5652,139 +5651,139 @@
       </c>
       <c r="C2">
         <f>'India Data'!I57</f>
-        <v>0.65902960122210263</v>
+        <v>0.66994176937584526</v>
       </c>
       <c r="D2">
         <f>'India Data'!J57</f>
-        <v>0.65552062800241451</v>
+        <v>0.67014897446969079</v>
       </c>
       <c r="E2">
         <f>'India Data'!K57</f>
-        <v>0.65086002903774454</v>
+        <v>0.67042418313769436</v>
       </c>
       <c r="F2">
         <f>'India Data'!L57</f>
-        <v>0.64470349652978387</v>
+        <v>0.67078772677744558</v>
       </c>
       <c r="G2">
         <f>'India Data'!M57</f>
-        <v>0.6366291704210667</v>
+        <v>0.67126451625241479</v>
       </c>
       <c r="H2">
         <f>'India Data'!N57</f>
-        <v>0.62613897962082321</v>
+        <v>0.67188396269248052</v>
       </c>
       <c r="I2">
         <f>'India Data'!O57</f>
-        <v>0.61267571752574523</v>
+        <v>0.67267896918333236</v>
       </c>
       <c r="J2">
         <f>'India Data'!P57</f>
-        <v>0.59566534696168016</v>
+        <v>0.67368343265694852</v>
       </c>
       <c r="K2">
         <f>'India Data'!Q57</f>
-        <v>0.57459367796989913</v>
+        <v>0.67492771606339508</v>
       </c>
       <c r="L2">
         <f>'India Data'!R57</f>
-        <v>0.54912053756382329</v>
+        <v>0.67643190663936359</v>
       </c>
       <c r="M2">
         <f>'India Data'!S57</f>
-        <v>0.5192197750299189</v>
+        <v>0.67819754858616665</v>
       </c>
       <c r="N2">
         <f>'India Data'!T57</f>
-        <v>0.48531084169992994</v>
+        <v>0.68019987327574238</v>
       </c>
       <c r="O2">
         <f>'India Data'!U57</f>
-        <v>0.44832714706418841</v>
+        <v>0.68238376281777591</v>
       </c>
       <c r="P2">
         <f>'India Data'!V57</f>
-        <v>0.40966666666666679</v>
+        <v>0.68466666666666676</v>
       </c>
       <c r="Q2">
         <f>'India Data'!W57</f>
-        <v>0.37100618626914517</v>
+        <v>0.68694957051555761</v>
       </c>
       <c r="R2">
         <f>'India Data'!X57</f>
-        <v>0.3340224916334037</v>
+        <v>0.68913346005759113</v>
       </c>
       <c r="S2">
         <f>'India Data'!Y57</f>
-        <v>0.30011355830341474</v>
+        <v>0.69113578474716686</v>
       </c>
       <c r="T2">
         <f>'India Data'!Z57</f>
-        <v>0.27021279576951029</v>
+        <v>0.69290142669396992</v>
       </c>
       <c r="U2">
         <f>'India Data'!AA57</f>
-        <v>0.24473965536343445</v>
+        <v>0.69440561726993844</v>
       </c>
       <c r="V2">
         <f>'India Data'!AB57</f>
-        <v>0.22366798637165336</v>
+        <v>0.69564990067638499</v>
       </c>
       <c r="W2">
         <f>'India Data'!AC57</f>
-        <v>0.20665761580758835</v>
+        <v>0.69665436415000115</v>
       </c>
       <c r="X2">
         <f>'India Data'!AD57</f>
-        <v>0.19319435371251037</v>
+        <v>0.69744937064085299</v>
       </c>
       <c r="Y2">
         <f>'India Data'!AE57</f>
-        <v>0.18270416291226688</v>
+        <v>0.69806881708091872</v>
       </c>
       <c r="Z2">
         <f>'India Data'!AF57</f>
-        <v>0.17462983680354965</v>
+        <v>0.69854560655588793</v>
       </c>
       <c r="AA2">
         <f>'India Data'!AG57</f>
-        <v>0.16847330429558904</v>
+        <v>0.69890915019563915</v>
       </c>
       <c r="AB2">
         <f>'India Data'!AH57</f>
-        <v>0.16381270533091907</v>
+        <v>0.69918435886364272</v>
       </c>
       <c r="AC2">
         <f>'India Data'!AI57</f>
-        <v>0.16030373211123095</v>
+        <v>0.69939156395748825</v>
       </c>
       <c r="AD2">
         <f>'India Data'!AJ57</f>
-        <v>0.15767264712603979</v>
+        <v>0.69954692969473964</v>
       </c>
       <c r="AE2">
         <f>'India Data'!AK57</f>
-        <v>0.15570588553948805</v>
+        <v>0.69966306709266179</v>
       </c>
       <c r="AF2">
         <f>'India Data'!AL57</f>
-        <v>0.15423909528554103</v>
+        <v>0.69974968115130309</v>
       </c>
       <c r="AG2">
         <f>'India Data'!AM57</f>
-        <v>0.15314705690796271</v>
+        <v>0.69981416608759139</v>
       </c>
       <c r="AH2">
         <f>'India Data'!AN57</f>
-        <v>0.15233506452824885</v>
+        <v>0.69986211428973111</v>
       </c>
       <c r="AI2">
         <f>'India Data'!AO57</f>
-        <v>0.15173187659498333</v>
+        <v>0.69989773257590593</v>
       </c>
       <c r="AJ2">
         <f>'India Data'!AP57</f>
-        <v>0.15128411562601229</v>
+        <v>0.69992417288986319</v>
       </c>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.45">
@@ -6087,139 +6086,139 @@
       </c>
       <c r="C5">
         <f>'India Data'!I60</f>
-        <v>0.34039215686274105</v>
+        <v>0.33270588235294074</v>
       </c>
       <c r="D5">
         <f>'India Data'!J60</f>
-        <v>0.35011764705881987</v>
+        <v>0.33474509803921482</v>
       </c>
       <c r="E5">
         <f>'India Data'!K60</f>
-        <v>0.35984313725489869</v>
+        <v>0.33678431372548978</v>
       </c>
       <c r="F5">
         <f>'India Data'!L60</f>
-        <v>0.36956862745097752</v>
+        <v>0.33882352941176386</v>
       </c>
       <c r="G5">
         <f>'India Data'!M60</f>
-        <v>0.37929411764705634</v>
+        <v>0.34086274509803882</v>
       </c>
       <c r="H5">
         <f>'India Data'!N60</f>
-        <v>0.38901960784313516</v>
+        <v>0.3429019607843129</v>
       </c>
       <c r="I5">
         <f>'India Data'!O60</f>
-        <v>0.39874509803921399</v>
+        <v>0.34494117647058786</v>
       </c>
       <c r="J5">
         <f>'India Data'!P60</f>
-        <v>0.40847058823529281</v>
+        <v>0.34698039215686194</v>
       </c>
       <c r="K5">
         <f>'India Data'!Q60</f>
-        <v>0.41819607843137163</v>
+        <v>0.3490196078431369</v>
       </c>
       <c r="L5">
         <f>'India Data'!R60</f>
-        <v>0.4279215686274469</v>
+        <v>0.35105882352941098</v>
       </c>
       <c r="M5">
         <f>'India Data'!S60</f>
-        <v>0.43764705882352573</v>
+        <v>0.35309803921568594</v>
       </c>
       <c r="N5">
         <f>'India Data'!T60</f>
-        <v>0.44737254901960455</v>
+        <v>0.35513725490196002</v>
       </c>
       <c r="O5">
         <f>'India Data'!U60</f>
-        <v>0.45709803921568337</v>
+        <v>0.35717647058823498</v>
       </c>
       <c r="P5">
         <f>'India Data'!V60</f>
-        <v>0.46682352941176219</v>
+        <v>0.35921568627450906</v>
       </c>
       <c r="Q5">
         <f>'India Data'!W60</f>
-        <v>0.47654901960784102</v>
+        <v>0.36125490196078403</v>
       </c>
       <c r="R5">
         <f>'India Data'!X60</f>
-        <v>0.48627450980391984</v>
+        <v>0.3632941176470581</v>
       </c>
       <c r="S5">
         <f>'India Data'!Y60</f>
-        <v>0.49599999999999866</v>
+        <v>0.36533333333333307</v>
       </c>
       <c r="T5">
         <f>'India Data'!Z60</f>
-        <v>0.50572549019607749</v>
+        <v>0.36737254901960714</v>
       </c>
       <c r="U5">
         <f>'India Data'!AA60</f>
-        <v>0.51545098039215276</v>
+        <v>0.36941176470588211</v>
       </c>
       <c r="V5">
         <f>'India Data'!AB60</f>
-        <v>0.52517647058823158</v>
+        <v>0.37145098039215618</v>
       </c>
       <c r="W5">
         <f>'India Data'!AC60</f>
-        <v>0.5349019607843104</v>
+        <v>0.37349019607843115</v>
       </c>
       <c r="X5">
         <f>'India Data'!AD60</f>
-        <v>0.54462745098038923</v>
+        <v>0.37552941176470522</v>
       </c>
       <c r="Y5">
         <f>'India Data'!AE60</f>
-        <v>0.55435294117646805</v>
+        <v>0.37756862745098019</v>
       </c>
       <c r="Z5">
         <f>'India Data'!AF60</f>
-        <v>0.56407843137254687</v>
+        <v>0.37960784313725426</v>
       </c>
       <c r="AA5">
         <f>'India Data'!AG60</f>
-        <v>0.5738039215686257</v>
+        <v>0.38164705882352923</v>
       </c>
       <c r="AB5">
         <f>'India Data'!AH60</f>
-        <v>0.58352941176470452</v>
+        <v>0.3836862745098033</v>
       </c>
       <c r="AC5">
         <f>'India Data'!AI60</f>
-        <v>0.59325490196078334</v>
+        <v>0.38572549019607827</v>
       </c>
       <c r="AD5">
         <f>'India Data'!AJ60</f>
-        <v>0.60298039215685861</v>
+        <v>0.38776470588235235</v>
       </c>
       <c r="AE5">
         <f>'India Data'!AK60</f>
-        <v>0.61270588235293744</v>
+        <v>0.38980392156862731</v>
       </c>
       <c r="AF5">
         <f>'India Data'!AL60</f>
-        <v>0.62243137254901626</v>
+        <v>0.39184313725490139</v>
       </c>
       <c r="AG5">
         <f>'India Data'!AM60</f>
-        <v>0.63215686274509508</v>
+        <v>0.39388235294117635</v>
       </c>
       <c r="AH5">
         <f>'India Data'!AN60</f>
-        <v>0.64188235294117391</v>
+        <v>0.39592156862745043</v>
       </c>
       <c r="AI5">
         <f>'India Data'!AO60</f>
-        <v>0.65160784313725273</v>
+        <v>0.3979607843137245</v>
       </c>
       <c r="AJ5">
         <f>'India Data'!AP60</f>
-        <v>0.66133333333333155</v>
+        <v>0.39999999999999947</v>
       </c>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.45">
@@ -11745,8 +11744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="E90" sqref="E90"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="G60" sqref="G60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -19057,8 +19056,7 @@
         <v>0.48900000000000005</v>
       </c>
       <c r="E53">
-        <f>MIN(1,D53*'India Assumptions'!$A$4)</f>
-        <v>0.97800000000000009</v>
+        <v>0.6</v>
       </c>
       <c r="F53" s="15" t="str">
         <f t="shared" si="6"/>
@@ -19070,139 +19068,139 @@
       </c>
       <c r="I53">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($H$7:I$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,I$7))</f>
-        <v>0.50338235294117339</v>
+        <v>0.49226470588235305</v>
       </c>
       <c r="J53">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($H$7:J$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,J$7))</f>
-        <v>0.51776470588234957</v>
+        <v>0.49552941176470622</v>
       </c>
       <c r="K53">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($H$7:K$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,K$7))</f>
-        <v>0.53214705882352931</v>
+        <v>0.4987941176470585</v>
       </c>
       <c r="L53">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($H$7:L$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,L$7))</f>
-        <v>0.54652941176470549</v>
+        <v>0.50205882352941167</v>
       </c>
       <c r="M53">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($H$7:M$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,M$7))</f>
-        <v>0.56091176470588167</v>
+        <v>0.50532352941176484</v>
       </c>
       <c r="N53">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($H$7:N$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,N$7))</f>
-        <v>0.57529411764705785</v>
+        <v>0.50858823529411801</v>
       </c>
       <c r="O53">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($H$7:O$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,O$7))</f>
-        <v>0.58967647058823403</v>
+        <v>0.51185294117647029</v>
       </c>
       <c r="P53">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($H$7:P$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,P$7))</f>
-        <v>0.6040588235294102</v>
+        <v>0.51511764705882346</v>
       </c>
       <c r="Q53">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($H$7:Q$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,Q$7))</f>
-        <v>0.61844117647058638</v>
+        <v>0.51838235294117663</v>
       </c>
       <c r="R53">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($H$7:R$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,R$7))</f>
-        <v>0.63282352941176256</v>
+        <v>0.5216470588235298</v>
       </c>
       <c r="S53">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($H$7:S$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,S$7))</f>
-        <v>0.64720588235293874</v>
+        <v>0.52491176470588208</v>
       </c>
       <c r="T53">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($H$7:T$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,T$7))</f>
-        <v>0.66158823529411492</v>
+        <v>0.52817647058823525</v>
       </c>
       <c r="U53">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($H$7:U$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,U$7))</f>
-        <v>0.6759705882352911</v>
+        <v>0.53144117647058842</v>
       </c>
       <c r="V53">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($H$7:V$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,V$7))</f>
-        <v>0.69035294117646728</v>
+        <v>0.53470588235294159</v>
       </c>
       <c r="W53">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($H$7:W$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,W$7))</f>
-        <v>0.70473529411764702</v>
+        <v>0.53797058823529387</v>
       </c>
       <c r="X53">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($H$7:X$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,X$7))</f>
-        <v>0.7191176470588232</v>
+        <v>0.54123529411764704</v>
       </c>
       <c r="Y53">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($H$7:Y$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,Y$7))</f>
-        <v>0.73349999999999937</v>
+        <v>0.54450000000000021</v>
       </c>
       <c r="Z53">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($H$7:Z$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,Z$7))</f>
-        <v>0.74788235294117555</v>
+        <v>0.54776470588235338</v>
       </c>
       <c r="AA53">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($H$7:AA$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,AA$7))</f>
-        <v>0.76226470588235173</v>
+        <v>0.55102941176470566</v>
       </c>
       <c r="AB53">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($H$7:AB$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,AB$7))</f>
-        <v>0.77664705882352791</v>
+        <v>0.55429411764705883</v>
       </c>
       <c r="AC53">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($H$7:AC$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,AC$7))</f>
-        <v>0.79102941176470409</v>
+        <v>0.557558823529412</v>
       </c>
       <c r="AD53">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($H$7:AD$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,AD$7))</f>
-        <v>0.80541176470588027</v>
+        <v>0.56082352941176516</v>
       </c>
       <c r="AE53">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($H$7:AE$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,AE$7))</f>
-        <v>0.81979411764705645</v>
+        <v>0.56408823529411745</v>
       </c>
       <c r="AF53">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($H$7:AF$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,AF$7))</f>
-        <v>0.83417647058823263</v>
+        <v>0.56735294117647062</v>
       </c>
       <c r="AG53">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($H$7:AG$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,AG$7))</f>
-        <v>0.84855882352940881</v>
+        <v>0.57061764705882378</v>
       </c>
       <c r="AH53">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($H$7:AH$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,AH$7))</f>
-        <v>0.86294117647058499</v>
+        <v>0.57388235294117695</v>
       </c>
       <c r="AI53">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($H$7:AI$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,AI$7))</f>
-        <v>0.87732352941176472</v>
+        <v>0.57714705882352924</v>
       </c>
       <c r="AJ53">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($H$7:AJ$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,AJ$7))</f>
-        <v>0.8917058823529409</v>
+        <v>0.5804117647058824</v>
       </c>
       <c r="AK53">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($H$7:AK$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,AK$7))</f>
-        <v>0.90608823529411708</v>
+        <v>0.58367647058823557</v>
       </c>
       <c r="AL53">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($H$7:AL$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,AL$7))</f>
-        <v>0.92047058823529326</v>
+        <v>0.58694117647058874</v>
       </c>
       <c r="AM53">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($H$7:AM$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,AM$7))</f>
-        <v>0.93485294117646944</v>
+        <v>0.59020588235294102</v>
       </c>
       <c r="AN53">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($H$7:AN$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,AN$7))</f>
-        <v>0.94923529411764562</v>
+        <v>0.59347058823529419</v>
       </c>
       <c r="AO53">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($H$7:AO$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,AO$7))</f>
-        <v>0.9636176470588218</v>
+        <v>0.59673529411764736</v>
       </c>
       <c r="AP53">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($H$7:AP$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,AP$7))</f>
-        <v>0.97799999999999798</v>
+        <v>0.59999999999999964</v>
       </c>
     </row>
     <row r="54" spans="1:42" x14ac:dyDescent="0.45">
@@ -19692,8 +19690,7 @@
         <v>0.66933333333333356</v>
       </c>
       <c r="E57">
-        <f>E50*'India Assumptions'!$A$31</f>
-        <v>0.15</v>
+        <v>0.7</v>
       </c>
       <c r="F57" s="15" t="str">
         <f t="shared" si="6"/>
@@ -19705,139 +19702,139 @@
       </c>
       <c r="I57">
         <f>IF($F57="s-curve",$D57+($E57-$D57)*$I$2/(1+EXP($I$3*(COUNT($H$7:I$7)+$I$4))),TREND($D57:$E57,$D$7:$E$7,I$7))</f>
-        <v>0.65902960122210263</v>
+        <v>0.66994176937584526</v>
       </c>
       <c r="J57">
         <f>IF($F57="s-curve",$D57+($E57-$D57)*$I$2/(1+EXP($I$3*(COUNT($H$7:J$7)+$I$4))),TREND($D57:$E57,$D$7:$E$7,J$7))</f>
-        <v>0.65552062800241451</v>
+        <v>0.67014897446969079</v>
       </c>
       <c r="K57">
         <f>IF($F57="s-curve",$D57+($E57-$D57)*$I$2/(1+EXP($I$3*(COUNT($H$7:K$7)+$I$4))),TREND($D57:$E57,$D$7:$E$7,K$7))</f>
-        <v>0.65086002903774454</v>
+        <v>0.67042418313769436</v>
       </c>
       <c r="L57">
         <f>IF($F57="s-curve",$D57+($E57-$D57)*$I$2/(1+EXP($I$3*(COUNT($H$7:L$7)+$I$4))),TREND($D57:$E57,$D$7:$E$7,L$7))</f>
-        <v>0.64470349652978387</v>
+        <v>0.67078772677744558</v>
       </c>
       <c r="M57">
         <f>IF($F57="s-curve",$D57+($E57-$D57)*$I$2/(1+EXP($I$3*(COUNT($H$7:M$7)+$I$4))),TREND($D57:$E57,$D$7:$E$7,M$7))</f>
-        <v>0.6366291704210667</v>
+        <v>0.67126451625241479</v>
       </c>
       <c r="N57">
         <f>IF($F57="s-curve",$D57+($E57-$D57)*$I$2/(1+EXP($I$3*(COUNT($H$7:N$7)+$I$4))),TREND($D57:$E57,$D$7:$E$7,N$7))</f>
-        <v>0.62613897962082321</v>
+        <v>0.67188396269248052</v>
       </c>
       <c r="O57">
         <f>IF($F57="s-curve",$D57+($E57-$D57)*$I$2/(1+EXP($I$3*(COUNT($H$7:O$7)+$I$4))),TREND($D57:$E57,$D$7:$E$7,O$7))</f>
-        <v>0.61267571752574523</v>
+        <v>0.67267896918333236</v>
       </c>
       <c r="P57">
         <f>IF($F57="s-curve",$D57+($E57-$D57)*$I$2/(1+EXP($I$3*(COUNT($H$7:P$7)+$I$4))),TREND($D57:$E57,$D$7:$E$7,P$7))</f>
-        <v>0.59566534696168016</v>
+        <v>0.67368343265694852</v>
       </c>
       <c r="Q57">
         <f>IF($F57="s-curve",$D57+($E57-$D57)*$I$2/(1+EXP($I$3*(COUNT($H$7:Q$7)+$I$4))),TREND($D57:$E57,$D$7:$E$7,Q$7))</f>
-        <v>0.57459367796989913</v>
+        <v>0.67492771606339508</v>
       </c>
       <c r="R57">
         <f>IF($F57="s-curve",$D57+($E57-$D57)*$I$2/(1+EXP($I$3*(COUNT($H$7:R$7)+$I$4))),TREND($D57:$E57,$D$7:$E$7,R$7))</f>
-        <v>0.54912053756382329</v>
+        <v>0.67643190663936359</v>
       </c>
       <c r="S57">
         <f>IF($F57="s-curve",$D57+($E57-$D57)*$I$2/(1+EXP($I$3*(COUNT($H$7:S$7)+$I$4))),TREND($D57:$E57,$D$7:$E$7,S$7))</f>
-        <v>0.5192197750299189</v>
+        <v>0.67819754858616665</v>
       </c>
       <c r="T57">
         <f>IF($F57="s-curve",$D57+($E57-$D57)*$I$2/(1+EXP($I$3*(COUNT($H$7:T$7)+$I$4))),TREND($D57:$E57,$D$7:$E$7,T$7))</f>
-        <v>0.48531084169992994</v>
+        <v>0.68019987327574238</v>
       </c>
       <c r="U57">
         <f>IF($F57="s-curve",$D57+($E57-$D57)*$I$2/(1+EXP($I$3*(COUNT($H$7:U$7)+$I$4))),TREND($D57:$E57,$D$7:$E$7,U$7))</f>
-        <v>0.44832714706418841</v>
+        <v>0.68238376281777591</v>
       </c>
       <c r="V57">
         <f>IF($F57="s-curve",$D57+($E57-$D57)*$I$2/(1+EXP($I$3*(COUNT($H$7:V$7)+$I$4))),TREND($D57:$E57,$D$7:$E$7,V$7))</f>
-        <v>0.40966666666666679</v>
+        <v>0.68466666666666676</v>
       </c>
       <c r="W57">
         <f>IF($F57="s-curve",$D57+($E57-$D57)*$I$2/(1+EXP($I$3*(COUNT($H$7:W$7)+$I$4))),TREND($D57:$E57,$D$7:$E$7,W$7))</f>
-        <v>0.37100618626914517</v>
+        <v>0.68694957051555761</v>
       </c>
       <c r="X57">
         <f>IF($F57="s-curve",$D57+($E57-$D57)*$I$2/(1+EXP($I$3*(COUNT($H$7:X$7)+$I$4))),TREND($D57:$E57,$D$7:$E$7,X$7))</f>
-        <v>0.3340224916334037</v>
+        <v>0.68913346005759113</v>
       </c>
       <c r="Y57">
         <f>IF($F57="s-curve",$D57+($E57-$D57)*$I$2/(1+EXP($I$3*(COUNT($H$7:Y$7)+$I$4))),TREND($D57:$E57,$D$7:$E$7,Y$7))</f>
-        <v>0.30011355830341474</v>
+        <v>0.69113578474716686</v>
       </c>
       <c r="Z57">
         <f>IF($F57="s-curve",$D57+($E57-$D57)*$I$2/(1+EXP($I$3*(COUNT($H$7:Z$7)+$I$4))),TREND($D57:$E57,$D$7:$E$7,Z$7))</f>
-        <v>0.27021279576951029</v>
+        <v>0.69290142669396992</v>
       </c>
       <c r="AA57">
         <f>IF($F57="s-curve",$D57+($E57-$D57)*$I$2/(1+EXP($I$3*(COUNT($H$7:AA$7)+$I$4))),TREND($D57:$E57,$D$7:$E$7,AA$7))</f>
-        <v>0.24473965536343445</v>
+        <v>0.69440561726993844</v>
       </c>
       <c r="AB57">
         <f>IF($F57="s-curve",$D57+($E57-$D57)*$I$2/(1+EXP($I$3*(COUNT($H$7:AB$7)+$I$4))),TREND($D57:$E57,$D$7:$E$7,AB$7))</f>
-        <v>0.22366798637165336</v>
+        <v>0.69564990067638499</v>
       </c>
       <c r="AC57">
         <f>IF($F57="s-curve",$D57+($E57-$D57)*$I$2/(1+EXP($I$3*(COUNT($H$7:AC$7)+$I$4))),TREND($D57:$E57,$D$7:$E$7,AC$7))</f>
-        <v>0.20665761580758835</v>
+        <v>0.69665436415000115</v>
       </c>
       <c r="AD57">
         <f>IF($F57="s-curve",$D57+($E57-$D57)*$I$2/(1+EXP($I$3*(COUNT($H$7:AD$7)+$I$4))),TREND($D57:$E57,$D$7:$E$7,AD$7))</f>
-        <v>0.19319435371251037</v>
+        <v>0.69744937064085299</v>
       </c>
       <c r="AE57">
         <f>IF($F57="s-curve",$D57+($E57-$D57)*$I$2/(1+EXP($I$3*(COUNT($H$7:AE$7)+$I$4))),TREND($D57:$E57,$D$7:$E$7,AE$7))</f>
-        <v>0.18270416291226688</v>
+        <v>0.69806881708091872</v>
       </c>
       <c r="AF57">
         <f>IF($F57="s-curve",$D57+($E57-$D57)*$I$2/(1+EXP($I$3*(COUNT($H$7:AF$7)+$I$4))),TREND($D57:$E57,$D$7:$E$7,AF$7))</f>
-        <v>0.17462983680354965</v>
+        <v>0.69854560655588793</v>
       </c>
       <c r="AG57">
         <f>IF($F57="s-curve",$D57+($E57-$D57)*$I$2/(1+EXP($I$3*(COUNT($H$7:AG$7)+$I$4))),TREND($D57:$E57,$D$7:$E$7,AG$7))</f>
-        <v>0.16847330429558904</v>
+        <v>0.69890915019563915</v>
       </c>
       <c r="AH57">
         <f>IF($F57="s-curve",$D57+($E57-$D57)*$I$2/(1+EXP($I$3*(COUNT($H$7:AH$7)+$I$4))),TREND($D57:$E57,$D$7:$E$7,AH$7))</f>
-        <v>0.16381270533091907</v>
+        <v>0.69918435886364272</v>
       </c>
       <c r="AI57">
         <f>IF($F57="s-curve",$D57+($E57-$D57)*$I$2/(1+EXP($I$3*(COUNT($H$7:AI$7)+$I$4))),TREND($D57:$E57,$D$7:$E$7,AI$7))</f>
-        <v>0.16030373211123095</v>
+        <v>0.69939156395748825</v>
       </c>
       <c r="AJ57">
         <f>IF($F57="s-curve",$D57+($E57-$D57)*$I$2/(1+EXP($I$3*(COUNT($H$7:AJ$7)+$I$4))),TREND($D57:$E57,$D$7:$E$7,AJ$7))</f>
-        <v>0.15767264712603979</v>
+        <v>0.69954692969473964</v>
       </c>
       <c r="AK57">
         <f>IF($F57="s-curve",$D57+($E57-$D57)*$I$2/(1+EXP($I$3*(COUNT($H$7:AK$7)+$I$4))),TREND($D57:$E57,$D$7:$E$7,AK$7))</f>
-        <v>0.15570588553948805</v>
+        <v>0.69966306709266179</v>
       </c>
       <c r="AL57">
         <f>IF($F57="s-curve",$D57+($E57-$D57)*$I$2/(1+EXP($I$3*(COUNT($H$7:AL$7)+$I$4))),TREND($D57:$E57,$D$7:$E$7,AL$7))</f>
-        <v>0.15423909528554103</v>
+        <v>0.69974968115130309</v>
       </c>
       <c r="AM57">
         <f>IF($F57="s-curve",$D57+($E57-$D57)*$I$2/(1+EXP($I$3*(COUNT($H$7:AM$7)+$I$4))),TREND($D57:$E57,$D$7:$E$7,AM$7))</f>
-        <v>0.15314705690796271</v>
+        <v>0.69981416608759139</v>
       </c>
       <c r="AN57">
         <f>IF($F57="s-curve",$D57+($E57-$D57)*$I$2/(1+EXP($I$3*(COUNT($H$7:AN$7)+$I$4))),TREND($D57:$E57,$D$7:$E$7,AN$7))</f>
-        <v>0.15233506452824885</v>
+        <v>0.69986211428973111</v>
       </c>
       <c r="AO57">
         <f>IF($F57="s-curve",$D57+($E57-$D57)*$I$2/(1+EXP($I$3*(COUNT($H$7:AO$7)+$I$4))),TREND($D57:$E57,$D$7:$E$7,AO$7))</f>
-        <v>0.15173187659498333</v>
+        <v>0.69989773257590593</v>
       </c>
       <c r="AP57">
         <f>IF($F57="s-curve",$D57+($E57-$D57)*$I$2/(1+EXP($I$3*(COUNT($H$7:AP$7)+$I$4))),TREND($D57:$E57,$D$7:$E$7,AP$7))</f>
-        <v>0.15128411562601229</v>
+        <v>0.69992417288986319</v>
       </c>
     </row>
     <row r="58" spans="1:42" x14ac:dyDescent="0.45">
@@ -20163,8 +20160,7 @@
         <v>0.33066666666666639</v>
       </c>
       <c r="E60">
-        <f>MIN(1,D60*'India Assumptions'!$A$4)</f>
-        <v>0.66133333333333277</v>
+        <v>0.4</v>
       </c>
       <c r="F60" s="15" t="str">
         <f t="shared" si="6"/>
@@ -20176,139 +20172,139 @@
       </c>
       <c r="I60">
         <f>IF($F60="s-curve",$D60+($E60-$D60)*$I$2/(1+EXP($I$3*(COUNT($H$7:I$7)+$I$4))),TREND($D60:$E60,$D$7:$E$7,I$7))</f>
-        <v>0.34039215686274105</v>
+        <v>0.33270588235294074</v>
       </c>
       <c r="J60">
         <f>IF($F60="s-curve",$D60+($E60-$D60)*$I$2/(1+EXP($I$3*(COUNT($H$7:J$7)+$I$4))),TREND($D60:$E60,$D$7:$E$7,J$7))</f>
-        <v>0.35011764705881987</v>
+        <v>0.33474509803921482</v>
       </c>
       <c r="K60">
         <f>IF($F60="s-curve",$D60+($E60-$D60)*$I$2/(1+EXP($I$3*(COUNT($H$7:K$7)+$I$4))),TREND($D60:$E60,$D$7:$E$7,K$7))</f>
-        <v>0.35984313725489869</v>
+        <v>0.33678431372548978</v>
       </c>
       <c r="L60">
         <f>IF($F60="s-curve",$D60+($E60-$D60)*$I$2/(1+EXP($I$3*(COUNT($H$7:L$7)+$I$4))),TREND($D60:$E60,$D$7:$E$7,L$7))</f>
-        <v>0.36956862745097752</v>
+        <v>0.33882352941176386</v>
       </c>
       <c r="M60">
         <f>IF($F60="s-curve",$D60+($E60-$D60)*$I$2/(1+EXP($I$3*(COUNT($H$7:M$7)+$I$4))),TREND($D60:$E60,$D$7:$E$7,M$7))</f>
-        <v>0.37929411764705634</v>
+        <v>0.34086274509803882</v>
       </c>
       <c r="N60">
         <f>IF($F60="s-curve",$D60+($E60-$D60)*$I$2/(1+EXP($I$3*(COUNT($H$7:N$7)+$I$4))),TREND($D60:$E60,$D$7:$E$7,N$7))</f>
-        <v>0.38901960784313516</v>
+        <v>0.3429019607843129</v>
       </c>
       <c r="O60">
         <f>IF($F60="s-curve",$D60+($E60-$D60)*$I$2/(1+EXP($I$3*(COUNT($H$7:O$7)+$I$4))),TREND($D60:$E60,$D$7:$E$7,O$7))</f>
-        <v>0.39874509803921399</v>
+        <v>0.34494117647058786</v>
       </c>
       <c r="P60">
         <f>IF($F60="s-curve",$D60+($E60-$D60)*$I$2/(1+EXP($I$3*(COUNT($H$7:P$7)+$I$4))),TREND($D60:$E60,$D$7:$E$7,P$7))</f>
-        <v>0.40847058823529281</v>
+        <v>0.34698039215686194</v>
       </c>
       <c r="Q60">
         <f>IF($F60="s-curve",$D60+($E60-$D60)*$I$2/(1+EXP($I$3*(COUNT($H$7:Q$7)+$I$4))),TREND($D60:$E60,$D$7:$E$7,Q$7))</f>
-        <v>0.41819607843137163</v>
+        <v>0.3490196078431369</v>
       </c>
       <c r="R60">
         <f>IF($F60="s-curve",$D60+($E60-$D60)*$I$2/(1+EXP($I$3*(COUNT($H$7:R$7)+$I$4))),TREND($D60:$E60,$D$7:$E$7,R$7))</f>
-        <v>0.4279215686274469</v>
+        <v>0.35105882352941098</v>
       </c>
       <c r="S60">
         <f>IF($F60="s-curve",$D60+($E60-$D60)*$I$2/(1+EXP($I$3*(COUNT($H$7:S$7)+$I$4))),TREND($D60:$E60,$D$7:$E$7,S$7))</f>
-        <v>0.43764705882352573</v>
+        <v>0.35309803921568594</v>
       </c>
       <c r="T60">
         <f>IF($F60="s-curve",$D60+($E60-$D60)*$I$2/(1+EXP($I$3*(COUNT($H$7:T$7)+$I$4))),TREND($D60:$E60,$D$7:$E$7,T$7))</f>
-        <v>0.44737254901960455</v>
+        <v>0.35513725490196002</v>
       </c>
       <c r="U60">
         <f>IF($F60="s-curve",$D60+($E60-$D60)*$I$2/(1+EXP($I$3*(COUNT($H$7:U$7)+$I$4))),TREND($D60:$E60,$D$7:$E$7,U$7))</f>
-        <v>0.45709803921568337</v>
+        <v>0.35717647058823498</v>
       </c>
       <c r="V60">
         <f>IF($F60="s-curve",$D60+($E60-$D60)*$I$2/(1+EXP($I$3*(COUNT($H$7:V$7)+$I$4))),TREND($D60:$E60,$D$7:$E$7,V$7))</f>
-        <v>0.46682352941176219</v>
+        <v>0.35921568627450906</v>
       </c>
       <c r="W60">
         <f>IF($F60="s-curve",$D60+($E60-$D60)*$I$2/(1+EXP($I$3*(COUNT($H$7:W$7)+$I$4))),TREND($D60:$E60,$D$7:$E$7,W$7))</f>
-        <v>0.47654901960784102</v>
+        <v>0.36125490196078403</v>
       </c>
       <c r="X60">
         <f>IF($F60="s-curve",$D60+($E60-$D60)*$I$2/(1+EXP($I$3*(COUNT($H$7:X$7)+$I$4))),TREND($D60:$E60,$D$7:$E$7,X$7))</f>
-        <v>0.48627450980391984</v>
+        <v>0.3632941176470581</v>
       </c>
       <c r="Y60">
         <f>IF($F60="s-curve",$D60+($E60-$D60)*$I$2/(1+EXP($I$3*(COUNT($H$7:Y$7)+$I$4))),TREND($D60:$E60,$D$7:$E$7,Y$7))</f>
-        <v>0.49599999999999866</v>
+        <v>0.36533333333333307</v>
       </c>
       <c r="Z60">
         <f>IF($F60="s-curve",$D60+($E60-$D60)*$I$2/(1+EXP($I$3*(COUNT($H$7:Z$7)+$I$4))),TREND($D60:$E60,$D$7:$E$7,Z$7))</f>
-        <v>0.50572549019607749</v>
+        <v>0.36737254901960714</v>
       </c>
       <c r="AA60">
         <f>IF($F60="s-curve",$D60+($E60-$D60)*$I$2/(1+EXP($I$3*(COUNT($H$7:AA$7)+$I$4))),TREND($D60:$E60,$D$7:$E$7,AA$7))</f>
-        <v>0.51545098039215276</v>
+        <v>0.36941176470588211</v>
       </c>
       <c r="AB60">
         <f>IF($F60="s-curve",$D60+($E60-$D60)*$I$2/(1+EXP($I$3*(COUNT($H$7:AB$7)+$I$4))),TREND($D60:$E60,$D$7:$E$7,AB$7))</f>
-        <v>0.52517647058823158</v>
+        <v>0.37145098039215618</v>
       </c>
       <c r="AC60">
         <f>IF($F60="s-curve",$D60+($E60-$D60)*$I$2/(1+EXP($I$3*(COUNT($H$7:AC$7)+$I$4))),TREND($D60:$E60,$D$7:$E$7,AC$7))</f>
-        <v>0.5349019607843104</v>
+        <v>0.37349019607843115</v>
       </c>
       <c r="AD60">
         <f>IF($F60="s-curve",$D60+($E60-$D60)*$I$2/(1+EXP($I$3*(COUNT($H$7:AD$7)+$I$4))),TREND($D60:$E60,$D$7:$E$7,AD$7))</f>
-        <v>0.54462745098038923</v>
+        <v>0.37552941176470522</v>
       </c>
       <c r="AE60">
         <f>IF($F60="s-curve",$D60+($E60-$D60)*$I$2/(1+EXP($I$3*(COUNT($H$7:AE$7)+$I$4))),TREND($D60:$E60,$D$7:$E$7,AE$7))</f>
-        <v>0.55435294117646805</v>
+        <v>0.37756862745098019</v>
       </c>
       <c r="AF60">
         <f>IF($F60="s-curve",$D60+($E60-$D60)*$I$2/(1+EXP($I$3*(COUNT($H$7:AF$7)+$I$4))),TREND($D60:$E60,$D$7:$E$7,AF$7))</f>
-        <v>0.56407843137254687</v>
+        <v>0.37960784313725426</v>
       </c>
       <c r="AG60">
         <f>IF($F60="s-curve",$D60+($E60-$D60)*$I$2/(1+EXP($I$3*(COUNT($H$7:AG$7)+$I$4))),TREND($D60:$E60,$D$7:$E$7,AG$7))</f>
-        <v>0.5738039215686257</v>
+        <v>0.38164705882352923</v>
       </c>
       <c r="AH60">
         <f>IF($F60="s-curve",$D60+($E60-$D60)*$I$2/(1+EXP($I$3*(COUNT($H$7:AH$7)+$I$4))),TREND($D60:$E60,$D$7:$E$7,AH$7))</f>
-        <v>0.58352941176470452</v>
+        <v>0.3836862745098033</v>
       </c>
       <c r="AI60">
         <f>IF($F60="s-curve",$D60+($E60-$D60)*$I$2/(1+EXP($I$3*(COUNT($H$7:AI$7)+$I$4))),TREND($D60:$E60,$D$7:$E$7,AI$7))</f>
-        <v>0.59325490196078334</v>
+        <v>0.38572549019607827</v>
       </c>
       <c r="AJ60">
         <f>IF($F60="s-curve",$D60+($E60-$D60)*$I$2/(1+EXP($I$3*(COUNT($H$7:AJ$7)+$I$4))),TREND($D60:$E60,$D$7:$E$7,AJ$7))</f>
-        <v>0.60298039215685861</v>
+        <v>0.38776470588235235</v>
       </c>
       <c r="AK60">
         <f>IF($F60="s-curve",$D60+($E60-$D60)*$I$2/(1+EXP($I$3*(COUNT($H$7:AK$7)+$I$4))),TREND($D60:$E60,$D$7:$E$7,AK$7))</f>
-        <v>0.61270588235293744</v>
+        <v>0.38980392156862731</v>
       </c>
       <c r="AL60">
         <f>IF($F60="s-curve",$D60+($E60-$D60)*$I$2/(1+EXP($I$3*(COUNT($H$7:AL$7)+$I$4))),TREND($D60:$E60,$D$7:$E$7,AL$7))</f>
-        <v>0.62243137254901626</v>
+        <v>0.39184313725490139</v>
       </c>
       <c r="AM60">
         <f>IF($F60="s-curve",$D60+($E60-$D60)*$I$2/(1+EXP($I$3*(COUNT($H$7:AM$7)+$I$4))),TREND($D60:$E60,$D$7:$E$7,AM$7))</f>
-        <v>0.63215686274509508</v>
+        <v>0.39388235294117635</v>
       </c>
       <c r="AN60">
         <f>IF($F60="s-curve",$D60+($E60-$D60)*$I$2/(1+EXP($I$3*(COUNT($H$7:AN$7)+$I$4))),TREND($D60:$E60,$D$7:$E$7,AN$7))</f>
-        <v>0.64188235294117391</v>
+        <v>0.39592156862745043</v>
       </c>
       <c r="AO60">
         <f>IF($F60="s-curve",$D60+($E60-$D60)*$I$2/(1+EXP($I$3*(COUNT($H$7:AO$7)+$I$4))),TREND($D60:$E60,$D$7:$E$7,AO$7))</f>
-        <v>0.65160784313725273</v>
+        <v>0.3979607843137245</v>
       </c>
       <c r="AP60">
         <f>IF($F60="s-curve",$D60+($E60-$D60)*$I$2/(1+EXP($I$3*(COUNT($H$7:AP$7)+$I$4))),TREND($D60:$E60,$D$7:$E$7,AP$7))</f>
-        <v>0.66133333333333155</v>
+        <v>0.39999999999999947</v>
       </c>
     </row>
     <row r="61" spans="1:42" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Remove 2-wheeler plug-in hybrids
</commit_message>
<xml_diff>
--- a/InputData/trans/MPNVbT/Max Perc New Veh by Technology.xlsx
+++ b/InputData/trans/MPNVbT/Max Perc New Veh by Technology.xlsx
@@ -30,7 +30,7 @@
     <sheet name="MPNVbT-motorbikes-psgr" sheetId="17" r:id="rId16"/>
     <sheet name="MPNVbT-motorbikes-frgt" sheetId="18" r:id="rId17"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterate="1" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -9588,135 +9588,135 @@
       </c>
       <c r="C6">
         <f>'India Data'!I82</f>
-        <v>5.9520917202232522E-3</v>
+        <v>0</v>
       </c>
       <c r="D6">
         <f>'India Data'!J82</f>
-        <v>7.9790980730597583E-3</v>
+        <v>0</v>
       </c>
       <c r="E6">
         <f>'India Data'!K82</f>
-        <v>1.0671356781790852E-2</v>
+        <v>0</v>
       </c>
       <c r="F6">
         <f>'India Data'!L82</f>
-        <v>1.4227761953270034E-2</v>
+        <v>0</v>
       </c>
       <c r="G6">
         <f>'India Data'!M82</f>
-        <v>1.889200681709895E-2</v>
+        <v>0</v>
       </c>
       <c r="H6">
         <f>'India Data'!N82</f>
-        <v>2.495180894817671E-2</v>
+        <v>0</v>
       </c>
       <c r="I6">
         <f>'India Data'!O82</f>
-        <v>3.2729046358683872E-2</v>
+        <v>0</v>
       </c>
       <c r="J6">
         <f>'India Data'!P82</f>
-        <v>4.2555319470146347E-2</v>
+        <v>0</v>
       </c>
       <c r="K6">
         <f>'India Data'!Q82</f>
-        <v>5.4727657141906902E-2</v>
+        <v>0</v>
       </c>
       <c r="L6">
         <f>'India Data'!R82</f>
-        <v>6.9442564950294702E-2</v>
+        <v>0</v>
       </c>
       <c r="M6">
         <f>'India Data'!S82</f>
-        <v>8.6715149212498815E-2</v>
+        <v>0</v>
       </c>
       <c r="N6">
         <f>'India Data'!T82</f>
-        <v>0.10630310813226136</v>
+        <v>0</v>
       </c>
       <c r="O6">
         <f>'India Data'!U82</f>
-        <v>0.12766724495650231</v>
+        <v>0</v>
       </c>
       <c r="P6">
         <f>'India Data'!V82</f>
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="Q6">
         <f>'India Data'!W82</f>
-        <v>0.17233275504349771</v>
+        <v>0</v>
       </c>
       <c r="R6">
         <f>'India Data'!X82</f>
-        <v>0.19369689186773861</v>
+        <v>0</v>
       </c>
       <c r="S6">
         <f>'India Data'!Y82</f>
-        <v>0.21328485078750117</v>
+        <v>0</v>
       </c>
       <c r="T6">
         <f>'India Data'!Z82</f>
-        <v>0.23055743504970527</v>
+        <v>0</v>
       </c>
       <c r="U6">
         <f>'India Data'!AA82</f>
-        <v>0.24527234285809307</v>
+        <v>0</v>
       </c>
       <c r="V6">
         <f>'India Data'!AB82</f>
-        <v>0.2574446805298537</v>
+        <v>0</v>
       </c>
       <c r="W6">
         <f>'India Data'!AC82</f>
-        <v>0.26727095364131614</v>
+        <v>0</v>
       </c>
       <c r="X6">
         <f>'India Data'!AD82</f>
-        <v>0.27504819105182327</v>
+        <v>0</v>
       </c>
       <c r="Y6">
         <f>'India Data'!AE82</f>
-        <v>0.28110799318290103</v>
+        <v>0</v>
       </c>
       <c r="Z6">
         <f>'India Data'!AF82</f>
-        <v>0.28577223804672996</v>
+        <v>0</v>
       </c>
       <c r="AA6">
         <f>'India Data'!AG82</f>
-        <v>0.28932864321820917</v>
+        <v>0</v>
       </c>
       <c r="AB6">
         <f>'India Data'!AH82</f>
-        <v>0.29202090192694019</v>
+        <v>0</v>
       </c>
       <c r="AC6">
         <f>'India Data'!AI82</f>
-        <v>0.29404790827977673</v>
+        <v>0</v>
       </c>
       <c r="AD6">
         <f>'India Data'!AJ82</f>
-        <v>0.29556779049201809</v>
+        <v>0</v>
       </c>
       <c r="AE6">
         <f>'India Data'!AK82</f>
-        <v>0.29670391721082207</v>
+        <v>0</v>
       </c>
       <c r="AF6">
         <f>'India Data'!AL82</f>
-        <v>0.29755122865405204</v>
+        <v>0</v>
       </c>
       <c r="AG6">
         <f>'India Data'!AM82</f>
-        <v>0.29818205955252475</v>
+        <v>0</v>
       </c>
       <c r="AH6">
         <f>'India Data'!AN82</f>
-        <v>0.29865111805171762</v>
+        <v>0</v>
       </c>
       <c r="AI6">
         <f>'India Data'!AO82</f>
-        <v>0.29899955780777598</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.45">
@@ -11744,8 +11744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP91"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="G60" sqref="G60"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="E83" sqref="E83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -23611,12 +23611,11 @@
         <v>0</v>
       </c>
       <c r="E82" s="10">
-        <f>E78*'India Assumptions'!$A$36</f>
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="F82" s="15" t="str">
         <f t="shared" si="8"/>
-        <v>s-curve</v>
+        <v>n/a</v>
       </c>
       <c r="H82" s="10">
         <f t="shared" si="7"/>
@@ -23624,139 +23623,139 @@
       </c>
       <c r="I82">
         <f>IF($F82="s-curve",$D82+($E82-$D82)*$I$2/(1+EXP($I$3*(COUNT($H$7:I$7)+$I$4))),TREND($D82:$E82,$D$7:$E$7,I$7))</f>
-        <v>5.9520917202232522E-3</v>
+        <v>0</v>
       </c>
       <c r="J82">
         <f>IF($F82="s-curve",$D82+($E82-$D82)*$I$2/(1+EXP($I$3*(COUNT($H$7:J$7)+$I$4))),TREND($D82:$E82,$D$7:$E$7,J$7))</f>
-        <v>7.9790980730597583E-3</v>
+        <v>0</v>
       </c>
       <c r="K82">
         <f>IF($F82="s-curve",$D82+($E82-$D82)*$I$2/(1+EXP($I$3*(COUNT($H$7:K$7)+$I$4))),TREND($D82:$E82,$D$7:$E$7,K$7))</f>
-        <v>1.0671356781790852E-2</v>
+        <v>0</v>
       </c>
       <c r="L82">
         <f>IF($F82="s-curve",$D82+($E82-$D82)*$I$2/(1+EXP($I$3*(COUNT($H$7:L$7)+$I$4))),TREND($D82:$E82,$D$7:$E$7,L$7))</f>
-        <v>1.4227761953270034E-2</v>
+        <v>0</v>
       </c>
       <c r="M82">
         <f>IF($F82="s-curve",$D82+($E82-$D82)*$I$2/(1+EXP($I$3*(COUNT($H$7:M$7)+$I$4))),TREND($D82:$E82,$D$7:$E$7,M$7))</f>
-        <v>1.889200681709895E-2</v>
+        <v>0</v>
       </c>
       <c r="N82">
         <f>IF($F82="s-curve",$D82+($E82-$D82)*$I$2/(1+EXP($I$3*(COUNT($H$7:N$7)+$I$4))),TREND($D82:$E82,$D$7:$E$7,N$7))</f>
-        <v>2.495180894817671E-2</v>
+        <v>0</v>
       </c>
       <c r="O82">
         <f>IF($F82="s-curve",$D82+($E82-$D82)*$I$2/(1+EXP($I$3*(COUNT($H$7:O$7)+$I$4))),TREND($D82:$E82,$D$7:$E$7,O$7))</f>
-        <v>3.2729046358683872E-2</v>
+        <v>0</v>
       </c>
       <c r="P82">
         <f>IF($F82="s-curve",$D82+($E82-$D82)*$I$2/(1+EXP($I$3*(COUNT($H$7:P$7)+$I$4))),TREND($D82:$E82,$D$7:$E$7,P$7))</f>
-        <v>4.2555319470146347E-2</v>
+        <v>0</v>
       </c>
       <c r="Q82">
         <f>IF($F82="s-curve",$D82+($E82-$D82)*$I$2/(1+EXP($I$3*(COUNT($H$7:Q$7)+$I$4))),TREND($D82:$E82,$D$7:$E$7,Q$7))</f>
-        <v>5.4727657141906902E-2</v>
+        <v>0</v>
       </c>
       <c r="R82">
         <f>IF($F82="s-curve",$D82+($E82-$D82)*$I$2/(1+EXP($I$3*(COUNT($H$7:R$7)+$I$4))),TREND($D82:$E82,$D$7:$E$7,R$7))</f>
-        <v>6.9442564950294702E-2</v>
+        <v>0</v>
       </c>
       <c r="S82">
         <f>IF($F82="s-curve",$D82+($E82-$D82)*$I$2/(1+EXP($I$3*(COUNT($H$7:S$7)+$I$4))),TREND($D82:$E82,$D$7:$E$7,S$7))</f>
-        <v>8.6715149212498815E-2</v>
+        <v>0</v>
       </c>
       <c r="T82">
         <f>IF($F82="s-curve",$D82+($E82-$D82)*$I$2/(1+EXP($I$3*(COUNT($H$7:T$7)+$I$4))),TREND($D82:$E82,$D$7:$E$7,T$7))</f>
-        <v>0.10630310813226136</v>
+        <v>0</v>
       </c>
       <c r="U82">
         <f>IF($F82="s-curve",$D82+($E82-$D82)*$I$2/(1+EXP($I$3*(COUNT($H$7:U$7)+$I$4))),TREND($D82:$E82,$D$7:$E$7,U$7))</f>
-        <v>0.12766724495650231</v>
+        <v>0</v>
       </c>
       <c r="V82">
         <f>IF($F82="s-curve",$D82+($E82-$D82)*$I$2/(1+EXP($I$3*(COUNT($H$7:V$7)+$I$4))),TREND($D82:$E82,$D$7:$E$7,V$7))</f>
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="W82">
         <f>IF($F82="s-curve",$D82+($E82-$D82)*$I$2/(1+EXP($I$3*(COUNT($H$7:W$7)+$I$4))),TREND($D82:$E82,$D$7:$E$7,W$7))</f>
-        <v>0.17233275504349771</v>
+        <v>0</v>
       </c>
       <c r="X82">
         <f>IF($F82="s-curve",$D82+($E82-$D82)*$I$2/(1+EXP($I$3*(COUNT($H$7:X$7)+$I$4))),TREND($D82:$E82,$D$7:$E$7,X$7))</f>
-        <v>0.19369689186773861</v>
+        <v>0</v>
       </c>
       <c r="Y82">
         <f>IF($F82="s-curve",$D82+($E82-$D82)*$I$2/(1+EXP($I$3*(COUNT($H$7:Y$7)+$I$4))),TREND($D82:$E82,$D$7:$E$7,Y$7))</f>
-        <v>0.21328485078750117</v>
+        <v>0</v>
       </c>
       <c r="Z82">
         <f>IF($F82="s-curve",$D82+($E82-$D82)*$I$2/(1+EXP($I$3*(COUNT($H$7:Z$7)+$I$4))),TREND($D82:$E82,$D$7:$E$7,Z$7))</f>
-        <v>0.23055743504970527</v>
+        <v>0</v>
       </c>
       <c r="AA82">
         <f>IF($F82="s-curve",$D82+($E82-$D82)*$I$2/(1+EXP($I$3*(COUNT($H$7:AA$7)+$I$4))),TREND($D82:$E82,$D$7:$E$7,AA$7))</f>
-        <v>0.24527234285809307</v>
+        <v>0</v>
       </c>
       <c r="AB82">
         <f>IF($F82="s-curve",$D82+($E82-$D82)*$I$2/(1+EXP($I$3*(COUNT($H$7:AB$7)+$I$4))),TREND($D82:$E82,$D$7:$E$7,AB$7))</f>
-        <v>0.2574446805298537</v>
+        <v>0</v>
       </c>
       <c r="AC82">
         <f>IF($F82="s-curve",$D82+($E82-$D82)*$I$2/(1+EXP($I$3*(COUNT($H$7:AC$7)+$I$4))),TREND($D82:$E82,$D$7:$E$7,AC$7))</f>
-        <v>0.26727095364131614</v>
+        <v>0</v>
       </c>
       <c r="AD82">
         <f>IF($F82="s-curve",$D82+($E82-$D82)*$I$2/(1+EXP($I$3*(COUNT($H$7:AD$7)+$I$4))),TREND($D82:$E82,$D$7:$E$7,AD$7))</f>
-        <v>0.27504819105182327</v>
+        <v>0</v>
       </c>
       <c r="AE82">
         <f>IF($F82="s-curve",$D82+($E82-$D82)*$I$2/(1+EXP($I$3*(COUNT($H$7:AE$7)+$I$4))),TREND($D82:$E82,$D$7:$E$7,AE$7))</f>
-        <v>0.28110799318290103</v>
+        <v>0</v>
       </c>
       <c r="AF82">
         <f>IF($F82="s-curve",$D82+($E82-$D82)*$I$2/(1+EXP($I$3*(COUNT($H$7:AF$7)+$I$4))),TREND($D82:$E82,$D$7:$E$7,AF$7))</f>
-        <v>0.28577223804672996</v>
+        <v>0</v>
       </c>
       <c r="AG82">
         <f>IF($F82="s-curve",$D82+($E82-$D82)*$I$2/(1+EXP($I$3*(COUNT($H$7:AG$7)+$I$4))),TREND($D82:$E82,$D$7:$E$7,AG$7))</f>
-        <v>0.28932864321820917</v>
+        <v>0</v>
       </c>
       <c r="AH82">
         <f>IF($F82="s-curve",$D82+($E82-$D82)*$I$2/(1+EXP($I$3*(COUNT($H$7:AH$7)+$I$4))),TREND($D82:$E82,$D$7:$E$7,AH$7))</f>
-        <v>0.29202090192694019</v>
+        <v>0</v>
       </c>
       <c r="AI82">
         <f>IF($F82="s-curve",$D82+($E82-$D82)*$I$2/(1+EXP($I$3*(COUNT($H$7:AI$7)+$I$4))),TREND($D82:$E82,$D$7:$E$7,AI$7))</f>
-        <v>0.29404790827977673</v>
+        <v>0</v>
       </c>
       <c r="AJ82">
         <f>IF($F82="s-curve",$D82+($E82-$D82)*$I$2/(1+EXP($I$3*(COUNT($H$7:AJ$7)+$I$4))),TREND($D82:$E82,$D$7:$E$7,AJ$7))</f>
-        <v>0.29556779049201809</v>
+        <v>0</v>
       </c>
       <c r="AK82">
         <f>IF($F82="s-curve",$D82+($E82-$D82)*$I$2/(1+EXP($I$3*(COUNT($H$7:AK$7)+$I$4))),TREND($D82:$E82,$D$7:$E$7,AK$7))</f>
-        <v>0.29670391721082207</v>
+        <v>0</v>
       </c>
       <c r="AL82">
         <f>IF($F82="s-curve",$D82+($E82-$D82)*$I$2/(1+EXP($I$3*(COUNT($H$7:AL$7)+$I$4))),TREND($D82:$E82,$D$7:$E$7,AL$7))</f>
-        <v>0.29755122865405204</v>
+        <v>0</v>
       </c>
       <c r="AM82">
         <f>IF($F82="s-curve",$D82+($E82-$D82)*$I$2/(1+EXP($I$3*(COUNT($H$7:AM$7)+$I$4))),TREND($D82:$E82,$D$7:$E$7,AM$7))</f>
-        <v>0.29818205955252475</v>
+        <v>0</v>
       </c>
       <c r="AN82">
         <f>IF($F82="s-curve",$D82+($E82-$D82)*$I$2/(1+EXP($I$3*(COUNT($H$7:AN$7)+$I$4))),TREND($D82:$E82,$D$7:$E$7,AN$7))</f>
-        <v>0.29865111805171762</v>
+        <v>0</v>
       </c>
       <c r="AO82">
         <f>IF($F82="s-curve",$D82+($E82-$D82)*$I$2/(1+EXP($I$3*(COUNT($H$7:AO$7)+$I$4))),TREND($D82:$E82,$D$7:$E$7,AO$7))</f>
-        <v>0.29899955780777598</v>
+        <v>0</v>
       </c>
       <c r="AP82">
         <f>IF($F82="s-curve",$D82+($E82-$D82)*$I$2/(1+EXP($I$3*(COUNT($H$7:AP$7)+$I$4))),TREND($D82:$E82,$D$7:$E$7,AP$7))</f>
-        <v>0.29925821305300959</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:42" x14ac:dyDescent="0.45">

</xml_diff>